<commit_message>
penambahan pada login dan approval cbs
</commit_message>
<xml_diff>
--- a/data/user-data-backup.xlsx
+++ b/data/user-data-backup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdul Aziz\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2BAC6E4E-DCEF-450A-BADA-63385FC74FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12280971-DD09-4FA9-804B-1F9BB528CE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="83">
   <si>
     <t>nip</t>
   </si>
@@ -37,9 +37,6 @@
     <t>Template</t>
   </si>
   <si>
-    <t>4224</t>
-  </si>
-  <si>
     <t>CECEP MULYANA</t>
   </si>
   <si>
@@ -52,9 +49,6 @@
     <t>TlQAEAwNAAAKAU5GVBACDQAACgFORlIl+AwZAAFoAfwB/AEAAP+pAQEfAAAAB/8cBxI9gBFJCoWFhYAPTgyGGLXAE08EnHa6QA1RDJOcPcEaUQKP91EhC0EQiGN5QQk+CIkHoiEOUhCG5aXhBjwFj4yu4RJODJqa0cEVUwWQH1GCFUsDkGVVgg1XG4KfZsIbTQKEmJLiFFIGjOC2YglDCJdjyqIOVCJ2og6DGk8GiFhBYw9RMH7VZaMISQSQIWlDEDJ3hFqNAw08D5ctpQMOLiGZ2ObDCjARg7bpYw80FohC8sMMG3OIk0rED0EKgpVShBdHCIgGUAECBzsB/z////////////8A/z8CCRgFA2IKCXgHAZEA/z//BPH/////AfICCSYFBkQA/y//////DfYKAoEJByMPBnH///8DAUYI/x//A/QFBxMM/48KDCUPCEQFAzcCCZEGDBkP/4//////A/MFAij/BPkKCxMMB2EC/38E/48NCxQMCXERDhIQDGQJCjT/DfQPCBkGB4ULDkIQEzIE/2//////EfQOC2QJC0L/DfYRGBkQDDIMEBMVE3L///8IB4QTDxMMCTgOETQSFTMLDRT/////G/kUDvEVExUPEHMOEWcUFvEQFRUX/0//////D/L/GP8WE/8SDv8RG/8XExUPEHMSGxQWGSEaGRH/FfIQFE8RGLEVGRH///////8TD0YUEfob/y8a/y8ZFiH///8XDxgWGBIa/x8ZGBIRG8P///////8UEfn/////////GvMBBB9xYxABBwDs4wz///8ABAAA/yAIFWAOJAV/E0UAEk0Ih55aIB0OCoiBfQAPTgyGdLrADFEMlRjBIBRPBZ+bMWEaUgKT/EWBC0MRi1+F4Qg+B4vkmUEHPQSQCaKhDlkPioiigRJPDJ2ZwUEVWAaSnt3hHSUEgSFZwhVSA5KgWmIbTQOIZV3iDFgZhpeGYhRWB4vmqqIJSAmYX8oiDlcdeKIGQxpPBYpSTeMOUSOD1V3jCEsEkh96wxArRYQsisMPJkSOW5XDDDwOlya14w0lJ5jc1iMLMA+IxN0DDzQdjgkthAsaJoGJPkQPRgyClkoEF0gJiYABAQP/BP///////wL/BQsqAwAv/////wL1////////DQb3BQGF/wD//wHyBQsYBwRS////AAPyBQsnBwhEDQv4CgORAf8vAgaBAQIX////DQ/2DAVxCwojEghx////BAVFCf8f/wT0BwoTEBZ4CBAYEv+P/////wTzDhMoEAhTBwQ4BQuRBwMoBQaJDA4TEAphAwVmBg1/Dw4TEAthBv///////w//Dgz/FBESEwpiDAY6D/9PBg1v/////xT1EQ50EgkYCAp1DhExExYxCwxVDg8nFBcoExBBEBMUFv8v////CQqFFhIUEAo4ERRFFRkzDg8V/////x/6FxGSGRYUEhNzERRnGBohExkUG/9P/////xLyHxwTGBUiExFYFP+fHBoSGRI6FREqFx8hGxYUEhNzFRgTGh0fHh0fGxkhExVBGBwhGRwTHf//////FhNDGBQbHx4i/xvzGhUR/////////xv/HB7/GxwyFx9U/////x3/FxQa/////////x70/xgJDkAPKgieE0HAEU4GpoOJoA9PDqpuvmAMTxC4GM4AFEgGwps1QRpSArcAOsELRhSyCqIhD1gTtYamARJODr2XyWEVVwe3Z1WiDVUhpyFh4hVQBLKgYqIbTQKnlIaCFFQIrOyJwgk9DLVfyqIOViicogIjGk4ErFZFQw9MRKLaVcMISAS09AbECxA7o41KxA9HDaKYTkQXRwmsELFEFCYHrpPGZBMiBqkgAQECEwP/X////////wQIOgL/PwD/H/////8A8wH/PwQHGQYDUv////8C8gQIFgb/PwwIRwcCgQH/P/8F8QH/L////wwLawkEgQcKOA7/f////wMENA0PNwr/XwYDNwQIgQYCKAQFeQkLEwoHYQIEdgX/jwwLFAoIcQ7/HwYHhQsNQg8SMhARGA0KJAkFSwz/TwX/b/////8Q9A0LZAgJRQsMJhAVGA8KMgoPFBL/P////wYHdBIOFAoHNw0QNBETMwsMFP////8V+RENcRMSFQ4Pgw0QZxUUIw8RFRP/X/////8O8xUUMf////8S9Q8RMRMRExAVsxf/H////xEQKf///////xYUQ////xf/HxQPGBX/TxQRFRb/H////////78aChLADykInxNJIBJOBal/feAOTg6pa8LAC0wQuRnWgBRHBsWZKQEaUQK5AzZhDEEUtYCWgRFGD78RpsEPVBK3lbkBFVcIuaFSIhtHAqtfXQINUR+pJW1iFk8DtPJ5QgoxDbOSeiIUUQmrXNYCDlUhnqTyohlQBK/bRUMJSAS2VVHjDkw+pRx14xArPqIhikMQE0ymJplDDzNGq346JA8nEaKaPqQWSQmrkr6kEiQFqQy9xBQjBrA4AQEHGwL/P////////wQHOgL/LwD/H////////wABMgQHGAYDUv////8C8gEHVwb/TwoHWAgCkQH/P/8F8QH/H/////8K9gkEcQgLSA3/f/8D9AIEVQYDNwQFiQkOFQsIYQ4PSAv/XwYCSQQHkQIEZgX/fwoMEwsHYQX/b/////8Q9QwJQQ3/HwYIhQkOYQ8RMRATHw4IIgkFOgr/TwsPFBH/L////wYIdAgJRQUMwhATLw8LQRENFAsIOA4QRRIWNgwKFf////8X+hMO8g8SFBb/f/////8N8v8R9A0Pcw4QZxMV/xcW/xQS/w8O/xD//xgWVBUR+BITLxAXoRb///8R/xIO/xQX//8R9xUQ/hkYEv///xMQ+v////8Z9BgWVBYUJRcZUf////////////8Y8RYUFBf/T/8eEj2gEUgKaIeFgA9MDGt2uiANTwt5F7nAE08GfZ05gRpRA3X5OkELSA5zZH0hCTkGcgmewQ5YDHHlpcEGOgV3j6VBEz0KgZjJgRVUB3VnUYINTxZpIFWiFU8FdqBmwhtLA22ZjsIUTAhz3rJiCUAHfWTGwg5PHWSiCmMaSwdwWD1jD0wjalRSgxAbQG/UYcMIRwN0L4lDEDZKfFiR4ww+D4A1qoMNIxqE1+LDCjAObrnlQw83FXJHAmQNGURwlkrEDz8JapVSRBdECXAPrQQUJgdzaAEDCToB/z////////////8A/z8DBxkFAlL/////AfIDCSYFBjQNCVgHAZEA/z//BPEA/y////8NDGsKA4EJByMPBnH///8CATUI/x//BfEDB4ML/48MECcLBlMFAjcDCZEGCxkP/4//////AvMFAygE/58KDBQLB3EBA3cE/48NDBQLCXH/CPkGB4UMDkIQDzERDhIQC2QKBEv/DfQE/2//////EfQODGQJDFL/EfH/FfgQCzILEBMWFHL///8IBocUDxMLCTkOETQSFjMMDRT/////HPkTDnEWFBUPEHMOE2EVFzEXFBYSChwOEWccFREQFhUY/0//////D/IZGiQXDzoTDhcRHJEYFBUPEHMSFRQXGhEaGBEUFmEQFTMcGTEXGhEb/y////8UD0YVESocGyL/GvIYFzH///8YFxEVGUIb/x8aGRIRHMMd//////8VERn///////8dG/P///////8bFf8c////HxJJIBJLB2uDeeAORQtrdrrADE4MfBjBQBRPBoGbKUEaUQJ5+jrBC0cOdGCJwQg8BHXjnUEHOwR4j53BEkMKgwqiQQ9aC3aZuQEVVAZ4n93BHSEHaGRZAg1WFmyfWoIbTANwIF3iFU8FeJiCQhRSCHPipsIJRwh+YMoiDlMYZKL+AhpOBnRTSQMPThlu1FUDCUcEeE5eIxAbS3UghgMRKT10W5mjDDoOgCeZAxAuL33c1kMLLw1ywdXjDjUZeggtZAsaIWmRQkQPPwtqlUbkFkcJcJO6xBIjBXh0AQMIKQH/L/////////////8A8gMJGQL/L/////8B8gMJKAUGRAsI9wkBkQD/L/8E8QD/H////wsO+goDcQgJJAwGgf///wIDRQf/H/8C9AUJEwz/fwYMGBD/j/////8C8wUDJwQLjwoPFQwJYQ8RSAwGUwUCSAMIkQIDVgQLfw0OEwwIYQT///////8N/w4K/xAHGAYJdQ4PMREUMQQLb/////8S9Q8OdBIVGA8JIgoEOg3/TwkKRQ4NJxIVJxEMQQwRFBcUcv///wcJhRQQFAwJOA8SRRMXMw4NFf////8d+hYPkhcUFBARcw8SZxUaERETFBf/T/////8Q8hcUJhMRFA8SeBYYIR0aExgTExUPKBL/n/8U9BARcxMYExoZERwaMRcUNxUPFxYdERgaUxwbL////xQXQRgSHB0cIv8Z8xcRFB7///////8Z/xoc/xkaIhId5B7/L/8b/xYSGv///////x4cVBwYJB3/X////////w==</t>
   </si>
   <si>
-    <t>4504</t>
-  </si>
-  <si>
     <t>MULYANI SUCIRATRI</t>
   </si>
   <si>
@@ -64,9 +58,6 @@
     <t>TlQAELANAAAKAU5GVBCmDQAACgFORlIlnA0ZAAFoAfwB/AEAAP+wAQEfAAAAB/wgBxGBoAdGC4aStsALTgiSfBGBBjgNlpslQRBBBIwGMgEFMAyXCG1hBEsOmSJ5ARA4B5QdeoESQQiRmwliDEUGoYZKIghOEZIjYkIUHASVJmmiDFUFoaedghUlBo1dqaIDQhaHo74CEEcCmE7iggQ0Mowb6aIFPGCQO/5iBTVylCESoxQnB4VLQqMCKBiRq0KjDkUDkipG4wU9E5enhYMIRQqar4njBjcNlJmSwwIXVYGoxeMNTgiQiQWEBCEKfJ4exAtOCJyXPWQSSAaJlnEEEEECk5V1hAlKC4uPsaQMPgWDBoABAwIVBP9v/////wHx////////AwgZAgBR////AAFVAwhVBQRBAf8f////BwYTBQKFCAk4Bf8v////AAJhCAkW////////BAYmCggnCQLEAQMzB/8vCgtLCAaSA/8f////AgNZBgp1DgsTCQVR/wX2BgjFCxY3EA1TDBQYDghVB/9P////FBUrEAmDCAY5Cg5xCv8f/////xLzDgtX/////wX6CRQ1DxMiCAcZChJSHBRjFguxE/8fDQUrCRBBERUSFxFBEw9BDQk1CxSFGBMi/w/xEAsZFBVh/xz4FA5SCgwz/////////w3yDxUTFxgxCw4jEv9fGRs3FhB1FxgTE/8/EQkYFBaBEAsqFBl0GxoWFxUhEQscFhshHhpVGBUx/xPxFRczGv8v////FA43/xzxHRtEGhaU/xjyFxtUHv8f////FhkUEh2xHx5E/xr0GRIY////////HRszGxQWHP8/////Hx5EGhYWGx1EH/8f////HhsUHf9P////////AQQoBYMFAAcABAAA8CMPiSAISQmKjq6AC04Ik3wVAQY6DJabGcEPRwWOCDZhBTINmgxp4QROD50ihWEQPgeWHIbhEkEIk5n9AQxIBqN0CgIDLQ6X9BpiASMHlYE+ogdPEpQsaqIUFgWVJ3UCDVQFpKmNIhUoBpCksqIPSQKdWrUiA0UTiEnqQgQ1Ko4h6SIGPFGSNApDBTtalioVIwYjM5kgIgMVJgiKqTKDDkUClVhSYwItHI4wUiMGNgyYqn0jCEUJmrGFowY4DZSnuaMNUQiRivnjAx8MfZ8WhAtNCJyZNeQRSgiLlWWkD0EEl5RpBAlJC4uNrSQMPgaEj95EEBcGfaQBAwgYAv9P/////wHx////////AwgZAgBR////AAFFAwhEBP8fAf8f////BggoBQBxCAs5Bf8v////AgMVCAsWCf9f////BAMnDA0oCAJiA/8vB/8vDA1bCAaSA/8f////BAM4BgxlDRQvCwVRCv8fBQFeCxInEP9fCRAVF/+P/////wX1CQUmAwjlDRk3EhBTDhYZDwZiB/9f////FhQvEgtzCAYoDA9xDP8f////FRY4DwhUCAcaDBVjHhZkEg2R////CglVCxIyERciF/8fEAknCxJRExgjFBPxERASCQt1DRZ1HBdD/xHyCxJhFBjxGBz/FxP/Eg3/Fhv//x74Fg9jDA5D////DQ8kFf9vGx04GRJ1/////xHxExg0HP8vGhwVFxFDFA37FhmRFA35FhtzIBxVGhgRGA0bGR0RIBxEFxEyDRZTFR6BHx00HBmD/xfyGh1EIP8f////GRsUFR/BIf9PIBpBGxUY/////yL1Hx0jHRYWHv8v/yLzISAzHBkVHR9DIf8f////IB0UH/8/Iv8f////HR9D/////////yHx4RcQjYAISwutjKLACk0JspoZwQ9HA7EQbWEFShLDIYLhEDIHsx2C4RI+B66W+kELOQm9fEICB0cZuAtlIhYPBK8kgUINTgW7p5FCFSYHqaC1Qg87BLhZvuIDMyCtqBFDDjsCty4iAxUlB5umeUMIPgm3qLmjDU0Js5X94wMgCpehFkQLSQi4nDnEEUgIrphtxA8/BLGVcSQJSAqmj8pkDDIGlBQBAgYZA/+P/////wHx////////AgYZAwCBAf8f////BAYpAwCBBgcW////////AAKICAn5BgByAv8vBf8fCAn7BgSRAv8f////AwEZBAp1CQ8vB/9P/wP2AQbkCQ0/DP8//w7/Cgv/BAX/////DQ//DAdjBgQpCgtxBQhP////DhA7CwZlBgQYCg5jEw1vDwnx/////wP6Bw0/DxH/CQv/Dv//EBL/Dwf//xD4DQvzCv8/////DAn/DRD/EhH/////DQv3DhOBFBJEEQ///wz/DxL/Ff//////DxD0DhSxFhVE/xH/EA4Y////////FBIzEA1PE/8/////FhJBEQ//EhREFv8f////FRIUFP9P////////jR0KkcAIRgqvi6LACk0JspoRYQ9IBLITceEFShHFIJJBETEHsxySYRM+B66U7gELOAm+dzpiBkEZuhtxIhYTBK+kecIUJgWqKJGiDU8Fu6Gp4g47BLlWvqIDNB2sJu2iBjhFsjgBYwQaRbIoDgMGGlKzqBFDDjQCtzAWQwUjVLMkIgMGITezDiZDFQgGmSRpwwENJKWPacMHEgi2qK1DDUsItaEK5ApECLidKQQRRwmvlV1EDz8GtJJlpAhECaaLvgQMMwWck+JEEBgEmFwBAQYZA/9/////////////////AgYaAwCBAf8f////BAYpAwBxBgcW/////wD3AQKHCQpJBgOGAv8v/wXyCAr7BgSiAv8f////AwEaBAmFChUvB/9f////AwZlChA/DQz0/xP/CQr/Bf//////Bf9PCP//ExY6CwZVEBX/DQfzBgQpCQthBgQYCRNTGBBfDQrx/////wP6Bw1PDhT/FQ//Dgz/Bwb/ChD//xT//wz/Bw3/DxH/EhQfEQ4fBw1vEBbzCgv/E///GBb/FQf/GhRf/w7/Bw1vDxIRFf//FBHxDw0fEBb0////FhCPCwkz/////////////w7/ERf/Eg3/ChD/Fhr//xT/ChBfExiBGRc0FBX/FRb0ExnBGxpU/xT/FhMY/////xz1GRcjFxAfGP8v/xzzGxpDFBX/FxlDG/8f////GhcVGf9PHP8f////FxlD/////////xvx/x8SgcAHQwltlLagC0wIdn4VYQY3DHydIQEQPQZ0A0UhBTEMggZpQQRKDH0igUEQOQh4HYmBEjUKem4CwgMuDXycDaIMQweE7jFCAScHfItKIgg+EHclaaIMUwWFXamCA0MQbaS6AhBJAn1P6kIENCBzGuniBTxKdzwCQwU0YHokDoMUJQtxqjqDDkEEfCtG4wVAEYBOSqMCMBR3p4mDCEQKgKyNAwc3DXyYkqMCFXJvp73DDU0Idp4exAtPCYCXPSQSRgdylF4kEDgEfZRxRAlHDHaRtYQMOQdrdAEDAhUF/4//////AfH///////8DCRkCAFH///8AAVUDC1oE/y////////8HBiMEAWEJCzgF/y////8CASYJCBUK/2////8EAygOCXcLAsQD/z//B/ISDnkJBpID/y////////8FAlkJC0ENClEEAzkG/38ODBMLCFQLDRUV/3//////CPEIBRYGDMMOFkcQClETFCsQC4MJBjn/DvH///8KCFULEDMPFSIJBxn/EvIbE2MQDJEV/x8KDWILEEERGBEXFEMRDxENCzUME4UYFSIPDRMQDBkTFGH/G/gTDlIH/3////8MDiMS/18ZGjcWEHUXGBMV/z8RCxgTFoH/////DfIPFBMXGDEQDCoTGXQa/x8XFCEUDBwWGiEd/18YFTP/FfEUFzMd/y////8ME2P/G/EcGjQYFnQWGRQSHLEe/08dGEIZEhj///////8cGiMZEzUb/y////8eGkEXFlYaHEQe/x////8dGhQc/0//////////HhCJQAhFB3OQqkALTAd4exHhBTcLe5wZoQ9BBnYJPYEFMQ2ECWnBBE0NgCKJgRA9CHodkcESOAp7nAVCDEcGhmkKQgMtDn/sJaIBJgl/hULCB04PeyZ14gxTBYhbtSIDQw9upbbCD0cCgiDpQgY8QHpK8gIENBx1NhIjBTo7fSkZQwYjJoCqLmMOPgN/L04jBjcMglxWQwIjFnapeSMIRAiCsoWjBjgNfaixYw1OCHifFkQLTQiCmTWkEUUIdZZaxA85BoCVacQIRg13j6kEDDsIbmgBAwgYAv9P/////wHx////////AwgZAgBR////AAFFAwtKBP8f////////BggoBAFRCAsoBf8f////AgMVCAsWCf9f////BAMXGgzICAJiA/8v/wfx/wz6CAaBA/8f////BAMoBv9vDBIvCwVRCv8f/wX1CAtCDf9fCw8WDf9P/////wnxCQUmAwjlDBY3Dw1TExIvDwtzCAYo/w7x////CglFCw8yEBUiCAcZ////GhNkDwyRFhIfEQ0SCQt1DBN1Ff8f/w3yCw9RERci/xXz/xDyCw9hEhTxFP//FRH/Dwv/Exj/DA4k////GhgzFg91F/8fFRFBEgz7ExaR/////xDxERQ0HP8/Egz5ExhzHP9fFxQRFAwbFhkRHP9PFRExDBNT/xrxGxk0/xbzFhgU/xvxHf9PHBVDGA4W////////GxkjGBM2Gv8v////HRlBFxZFGRtEHf8f////HBkUG/9P////////</t>
   </si>
   <si>
-    <t>3694</t>
-  </si>
-  <si>
     <t>RUSTY ARI MEI MANALU</t>
   </si>
   <si>
@@ -79,9 +70,6 @@
     <t>TlQAEAwNAAAKAU5GVBACDQAACgFORlIl+AwZAAFoAfwB/AEAAP+pAQEfAAAAB/UeBytKwBw3BKaQZsAXThCQ5rmgDEkFqCi6IBdBEI9lvcARShWVq77AHiYCqd0JoQhLBJPwGqEPTguNEl6BEVQjgCuCYRVQDI57lSETLiWBB6khESoqea7CgRxPAqIo6YESQyp/q+2hF1QCrd8+wghGBoCrjiIYWg2ZPZGiEhg+jGGiogxMBImnvcIaWAqLjcqiFC0tiZveYhZJEovfAWMMQAiQmgljG1QIg5UqQxlTBofiNuMIOwmO6FqDD1EIhYKSIxdVD3WNoqMaQAp39bnDEEcPdgZoAQUDFwH/X/////////////8A9QwDEgQCQwQHRQsP9gb/L////w4JVQT/L/8B8gD/fwL/T////wMMJQgHQQD/H////xMM5gMBdQIHJhIPx////////wMIIgsP8QYCZf8E8QoLHw8GGAcEJAMJURANFAoIIf8D9f8O8QYIkQMJcg4QMQ0LPw4N/xIP/wYI/wMK/wX/b////xMQZw4DYRES8g8LTwgKQw4QUgMFXQz/bxARLw0JUQsS9BYZdf////8G9w4MJ/8T8RgVMxQNQhoW/xIL/w0O/xUU//8P9AYNwhEU9hoWYg4MFv///xcYJBUQQREN8hATRRUbFBoSFQ0QExMXQhgbFBoUEREa9B3/fxn/Hw8SchMMJ/////8c9BgVIhUTFBf/Lxz/LxsaMhYaFP///////w8SURUbEh3/PxkWRBIUYRoVJBj/Pxz/H/8d8RUYMv////////8b8Rv/H////xkacxQVVQEEYF2iEAEHALSCE////wAEAAD/HixWAB03BKmMWmAXTRKP6LHADEgFqayygB4mAqsqwmAXRQ6SY8VAEUsSmN79AAlOBJf1DuEPUgyPHFYBEkkmgW2JYRIlLX4piqEVUQuTG6XBESEve6+yIRxQAqao3UEXUAOtLPUBE0cchd8yIglLBYNffWIQIByCXX0iESo4hK1+whdbDJxhrkIMTQSKqbViGlgLjqfS4hVMF4zf9cIMQQeQnP3iGlUIh5MiAxlSB4nhKiMJPQeM7E7jD1EIhn+KgxZWD3WQmiMaQwp4+qkjEUQOd2gBAwQYAf9v/////////////wD2AwRjBQJCBQc1Cw/2Bv8f////AP8f////FAzHBAGGDQpWBf8vAf8/AAyBBgJD////BAwkCAdBAgcWEw/H////////DAhzEA/yBgJl/wXxCQsfDwYoBwE4BAph/wfzCAQXCg0iDgsvDQ4UCQghAQSGDP9/DhH/Dwb/Bwn/Cg3/A/9/////FBJoDQRhCgMdDP9vEhEvDglCFREfDwI6Cwr0DRJCCxD/ExlW/////wb3Ew//Bw7/DRH/HRr/ExD/Bw7/DRX/Gxr/DQwo/xTxGBVEEQ7y////DwtfEBX3FhkhDQwW////FxgUFRJBDhIUFBhBGx1VGhEvEBr0Hf9vGf8fEw4jFAwX/////xz0GBUiFRQUF/8v/xzzGxpCFhoV////////DxNhG/8/Hf8/GRZUEBXyGhU1GBdFHP8f/x3xFRhD/////////xvxHP8f////GRpzFRtR/hmJXmAXRhey6Z4gDTkHwF3eABE9GbYr3WAXOxK13gHhCEwCsuwSIRBLFLAZXoERUTCjKKbhFVMLtq2mIRxNA8il2WEXUgTJKeohEz8jpt8+wghIBaFTXkIRMV2jrHbCF1sMvV+qYgxOBKiptYIaVg2ui86CFCs/q6jNYhZBGK+dCUMbVAmlkSbjGFQHp94uQwk8B6/vVqMPTQmogJZjF1YPlYyiwxpACpb4ucMQSA6ZLAH/////////A/MFAlQAAiQKBJH///////8EAVT///8AA0IGBTEHBlUC/y8A/z//CPEBBRYMC9f///////8DBjIKC0EEAWX/AvEKDCULBBgFAiMDB1ENChMLBkEAA3UICWEA/x////8PDWcJA2ED/18I/28NESYKB0EQDCMLBDoGByMJDUEKDDUO/0//////BPcOCxUEBtUKDTUQFRIJCCf/D/ETETMMClH///8LBkQMEBQVFFEJ/x////8SEyQRDUEMChINEUETFhQVDhQJDWMPE0EWGFYQDBIPCCf/////F/QTESIRDRMS/y8XFiMYFUEMFRT///////8LDlEW/y8Y/z8UDkUMECEVESUT/z8X/x//GPERE0L/////////FvEW/x////8UFXMQEVa4HIROABdGGrLsjqANNQjBLeHAFzsPuWDmgBBAFrXf9UAJSgK0BAKBECUYsSBeIRJFNqKunsEbSgLKJapBFk0KuqPRARdOBsYp9mETPhyo3zIiCUwFo1ti4hAfTqKsYkIXWgjBWGaCERxRpV2GYg8wCaKolgIeGQyorKkCGlYNsWK6AgxPBKmqxeIVPxyw3doiDTMGraD5ohpVCqiMFmMYTwmp3x7DCUEHrvNK4w9PCad8jsMWVxCWjZojGkMKmPutYxFFDphQAf////////8C8wUDVQADNQoEof///////wgGVQP/LwD/P/8H8QQBVf///wIHNgYFQQEFFgwL1////////wgGMwsEJv8D8QACUgoMNgsEKAUAOAIIUQD/L////xANOAkCYQkOGAoGQQAChQcQdAgCFAcQYw0TJQoGQRMOFAsESgYINAkNQgoPRhL/X/////8E9w8LFgQK1AkOgRYYRAkHKBARURYTQw4KYg8MIQQK1AkNhhMYIxQLFgQG1gwTFBsYhQf/P/////8V9BENNQn/HxD/PxUWFBMNMf///wsGVQ8UIhgXYQoNExEWMRkYUhQOQg8TFBj/Xxf/HxIGJxEHFxD/T/8a9BYTIRMNFBEVQv8a8xkYQhQYFf///////wsSYRkbM////xcUVQ8TUhgTNRYVRRr/H/8b8RMWQxD/j/////8Z8Rr/H////xcYcxMZUdUdK0KgHDcFiJJeoBdNDnUoukAXQQx2Z8HAEUcSeOTFQAxEBIjdCaEISgZ47hLhD0wLcwtagRE5HWiGgqETJxxnK4phFVEJdgmpIREpJGOtvmEcTgKEJ+mBEkMia631wRdTA43ePsIISgdqXHrCDzkMbqqKIhhZDX1CkkITGiR2YaqCDEwFcqa5ohpXCXPaxQISFxpsjMZCFCo+b5zaIhZFEnLfAWMMPQh3mglDG1AIapYqAxlOB3DmWoMPTQhthpZDF1APX/WioxA4DWNcAQsCZwH/X/////////////8A9QsCEgMEQwsJFQP/LwEAJ////wT/T////wILJQcGQQMGRQoOlgX/L////wQGJg8O1////////wIHIgoOQQUEZf8D8QgKEg7/HwYDJAL/XwcDFQIJYQ0RJQwKMRAMFAgHEQECdQsNYQwRIw8OQgQHkgIIgQD/b////xMQZw0CYREPIw4KQgcIQw0QUgIAXQv/bxARJwwJUQoPJRL/T/////8F9xIOFQUM0w0RghQX8Q0LJ/8T8RkWMxUMQhQS9Q8MIg0QdBYVEf8O9AUMwg8UHxoXYg0LFv///xgZJBYQQREV/xsa/xcS/w8M/xEMEg0QdBYbFBoUHxEQExMYQhn/HxoVERQa9Bz/b////w4SchMLJ////////xkWIhYTFBj/L/8b8xwUPxYbEhz/L/8X9BIUbxoWJBn/P/////8c8Rv/H/////8a8hQW9P8dK0rAHDgEi49WQBdNEHXmuYAMSQWKKcJgF0EKemTFQBFJD3zd/QAJTAV88wpBEEsNdRpSIRJTH2l7egETLSFnLI7BFU8IfBahoREyI2avskEcTgKIrOlhF1MDkCv1IRNHE3DeMkIJSwVtWn0CESk1ca1+whdaC4FdgoIPKwhvqLFCGlcKdWG2IgxMBnWnzsIVSxVy3vXCDD0IeJr94hpTCG6TGqMYUwhz4R7DCUEHc+hO4w9OB2+BiuMWUxBgkJpDGkAKZPWiAxE4D2NcAQsDeAH/b/////////////8A9gsDIwQCQgQGNQoOhgX/H////wsJFgT/LwEAOP///wL/P////wMLJAcGQQIGFhEO1////////wMHMwoOQgUCZQQBFQgKEg4FKAYBOAMJYQUHgQMAfgkMIg0KMRANJAgHIQMAbgsMcQ0PHw7/LwYHQggJEgD/f////xIQaAwDYQMAXQv/bxAPLw0JQRQPHw4COgoJFAwQQgoRJhP/X/////8F9xMR/wUN/wwU/xoZ/wwLKP8S8RcURA8N8hMOJgUN0wwPnxwVcQwLFv///xYXFBQQQf///w4KUxEUJxUYIQ0QFBIXQRocVRkPLw8a9xn/Txj/HxMRIRILF/////8b9BcUIhQQFBb/LxsaNBwZQhUZFf///////w4TYRcaIxz/P/8V9BEUUhkUNRf/Txv/H/8c8RQXQ/////////8a8Rr/H/////8Z8w8U9Q==</t>
   </si>
   <si>
-    <t>4670</t>
-  </si>
-  <si>
     <t>EKO RESTIOWATI</t>
   </si>
   <si>
@@ -91,9 +79,6 @@
     <t>TlQAELUMAAAKAU5GVBCrDAAACgFORlIloQwZAAFoAfwB/AEAAP+aAQEfAAAAB/8gB3oVwA0pA4h+FeAUMwKE9H7ABjMGeffJQAtZBIQG3qAWVQaAEC1BHTsKhPtiYQ9ZA4Z1aYEJVwKK9aZhBE4DjGjRwQETBJIT3qEWVgiNcA0iA0oGmRodohxRB4ZrKsIFWAiccT7CCk4EoQpC4hBYCY2UcWIYUgaI8IKCBUQFoP+yQgxcC5mIwiISVAuOJNViHR4DifL2YgdaBpOHRaMRWAqIaEmjA0wDje+lYwhVBYD2+sMKVgd/aQEkCFAFfZQexBJTDIFiIqQCLwSNg4JkEEsbfPnlpAtFDHfqBiUHTQl1BoAB////////AQoeAwJRAP8f/////wT2BgOUAQMTCP9//////wDxBAYlBwhVAv8/AAFUBQoXDwazAAF2/////wz3CgRxAf+P////Cg83DghhBwMVAQST/wL3AwRTBg8YDghxBg0UCwk/////Agdx/////wL/CAv/Ef//EBY8Dw5DBgQ3BQxx/wn/CAc0DRElF/+v/xT0EApRBAV3/////wvyCAdFDhInEf8vDQgmBwZ2DxIUGBGhFBMjEg4xBwaHBAq0CgU7DP9fFBstEw9RDhUUF/9f/wv1DQcnExsZGBVhEQ5EBg+jDg9DChCF/xb0GBJh/xv+ExBiDP9P////Fhk4GBdR/xH0DRJxEhNEEBSa/xv1GRhS////CxWhEhglHP9fFhkjGhwx/xf1FRJWGx0THv9vGhgTEhaVHBcnGBI5GR0UHv9/EhaVFP/v////HRky////CxflGh4pH/9/GRI9G/8//////x7y/////x/xHBqXGR1iHv8f/////xz3GhlUAAQABwAEAAD/H3gVQA0pBIh9FWAUMwKH9HpABzYFfPjFwAtZBIYF5iAXVQWCFjnBHTsKhf1a4Q9bBIh1cQEJVwOO9aLhBFQDjxXmIRdZCI5sEcICTAabHykCHVMIh2w2QgVXCJ1xRkIKTwSkCkZiEVgKj5JlIhhXBovxesIFQwWiAa7CDFwKmIW6ohFVC5Ax4cIdHQOL9O6iB1oGloQ9AxFUC4xkVSMDUgOQ8Z3jCFgFg/vuQwtaCYJpDaQHUgR/kRJEElMNg2UuJAIpBI98dsQPShp+/d0kDEIOeOv2pAdPCXZ0Af///////wEGGgMCQQD/H/////8E9gYDkwEDEwf/f/////8A8QQGJQcIRQL/PwABQwUJGA4GxAABdv////8L9gkEcQH/f////wkOSA0HcQIDhQEElP///wMEQwYOGA0IcQYNFwwKU////wIHgRMPIw4NVAYESAULcf////8I8w0MQhb/nxMaPg8JQQQFdv////8K8ggHVQ0ROBD/PxAIFwcGdw4RJRcUpRMSJBENQgcGiAQJxQYJYwv/TxMaHRIOUQ0UFRb/X/8K9QwGNxIVFBcUYRANVQYOtA0OVAkPlf8a+hURQf8a/hIPYQv/P////xUYORcWUf8Q9Q0RUREOSBITSf8a9RgXUf///woQlRQXFBkbZRUYExkbIRYKTRQRVhocJB0ZYRYXcxEVpRsWJhQXchgdFh7/XxEVpQ//3////xwYQv///woW5RkeKP///xkYRBoTTv////8d8v////8e8RsYlhUcsh3/H/////8b+BkYVf8Z9H7gBjEClvjFYAtXA6kF4qAWVAemDzVhHTsKqv9ewQ9YBa1zbSEJUwGz9KIBBVIDthjmYRdXCrRwGaICRwi5GR2iHFQIrGkyQgVUCcENRsIRVAy6kGXiF1YIsQSu4gxZDMODvmIRTg249e4iCFUHvYNBQxFYDrJnVSMDTwO086GDCFcFqPz24wpbC6ZpAUQIUASikCKkElQPpICKZBBMH6D91kQLPwyZ6woFB00JlCwBAQQ3Bf9/////////AgQlBQZVAP8/////Awf3CwSzAP9f/////wn/BwT/Av//////Bws3DQWhAAF1/wLz////Af9fBA0bDwaxBA0aCghD////AAVx/wzzCwRDAQKXAwnx////AAajCg8pEf+v/xX+DAdRAgN//////wjyBgVFBA1GDxFn/w7zDQozBQSHBwxBBAdjCf9f/xX9EAuRDhUZEg9hCgVrBAujDQQaCww1/xD0Ew+RDhMYEhFR/wr2BQ2xDQ5ECwmN/xX1ExJS////CAqnDxIVGP/PFRMzFP8/EQheDw1WFRYTFxRRERJzDRCV/xH3EhA1ExYUF/9vDRCVCf/v////FhMyEw09Ff8//////xfx/////xjx/xT2ExZRF/8f////////FBNU6Bt9GWATNAKk9HqABzYCmvjF4AtYA6sG5gAXVAenAFphEFwFr3F5gQhSAbbwnqEFTwO4Ge7hF1UKs2wdAgJHB7oeLQIdUgirbD7iBFMJwXNOwglJBMsPTiISUQ27jVVCF1AJtfNu4gY8BscCrkINWQvDgrbCEE8MuvjioghYCMCDQYMQVQ+1ZGHDAk8DtPWZIwlTBqsA8mMLUw2paRGkB1IEo4sSZBJREKV7fsQPSCCiA9LkCzsQm+z6hAdPCJVEAf////////8D/wQC/wAC8wX/f////////wMEJQUGRQH/P/8A//8H+AwExAEAb////wcMSAsFcQEChQAD9P///wECdAQPGwsGcQULFwoIU////wEChf8N8wwEVAIDmP8J8f////8G8wsKQhP/n/8X/g0HQQP/f/////8I8gYFVQsOMxP/fw4GFwUEdxAPVRETVf8S9xALQwUEiAcNUQQHY/8J9P///xIMgQsRFRQTlf8K8wYEdxASFBQRYQsFWwQMtA8EGwwNRf8X+hIRQRAVGRQTUf8O9QsPUREQNAwJfP8X9RUUUf///wgOlREUFBr/zxcVMxb/LxMKSxESURcYJBoWURMUcxIJXv8T9hEUchUZFhr/XxQSNQ3/3////xgVQhYVRBIXlP////8Z8v////8a8f8V9hcYYhn/H////////xYVVf8b9slAC1QFagbewBZRBmkPLUEdOQtt+l6hD1cDbXVtQQlWBHH1psEETgRyE+YhF1cJc24JIgNOBX4bGaIcUwhtbSrCBVcHfnE6wgpLBIIKQkIRVwlylm1CGFUHcO55AgU/BYL+skIMWwt8h74CElMKdPH2YgdYBniJRYMRVglvZU1jA1EEdO+lYwhTBmj0+sMKUwZsaQFECE4GZZcixBJRC2hkKkQCLAd1iIaEEEgWZ/TppAs/CmDsBuUGSgpgRAEBAyUEBVX///////8CBvcLA7P/////////CP8GA/8B//////8GCzcKBWEEABX/AfP///8AAVMDCxgKBXEDChYH/z//////BPH/DPMLCkMDATcCCPH/////BfMKCUIS/6//Fv4MBlEBAn//////B/IFBEUKDicQDXIJBSYEA3YLDxQOEET/D/MOCjEEA4cBBrQDBmMI/1//Fv0PC1EKEBUS/2//B/UJBCcPFhkTEGENClQDC6MKC0MGDIX/EfQTDmERFDgTElH/DfUJDnEOD0QM/5//FvUUE1L///8HDaYQExUaF8URFCMVFzH/EvUQDlYWGBMZ/28VExMOEZUXEicTDjkUGBQZ/38OEZX///////8YFDL///8HEuUVGSka/38UETkW/z//////GfL///////8aFRcUGGIZ/x//////F/cVFFT/GffF4AtUBW0F5kAXTwVr/1ohEFgDcHZ1wQhWBHX1nkEFUgR1FOqBF1YJdXAZwgJMBYMcKeIcUAhtbTZiBVcIgHNGYgpPBIcKSsIRUwh2k2HiF1UGdO91YgU/BIUArqIMWwp8hLqCEVQKd/PuwgdXBnuGPQMRVwlyYlkDA1AEd/GZAwlWBWz38kMLVwduag3EB08FZ5QWZBJRDGqAegQQSRZp+tkEDEIMYuv+ZAdKCmIsAQECJQMERf////////8F+AoCxP///////wUKSAkDcf8A9f8B9P///wABQwINGwkEcQIJFwgGU/////8D8f8L8woJVAIBSP8H8f////8E8wgMJBH/n/8V/gsFQQH/f/////8G8gQDVQkNOAz/LwgENwMCdwoNJRIPpf8O9BINpAMCiAELwQIFYwf/T/8V/Q4KUQkPFRH/X/8G9AgDJg4QFBIPYQwJVQIKtAkKVAULlf8V+RANQRATORIRUf8M9QQNwQ0ORAsHjP8V9RMSUf///wYMlQ8SFBT/bxATExT/LxEGTQ8NVhUWJBcUYREScw0Qpf8R9g8SchMXFhj/Xw0QpQf/7////xYTQhMSRxX/T/////8X8v////8Y8f8U9hMWYhf/H////////xQTVQ==</t>
   </si>
   <si>
-    <t>3947</t>
-  </si>
-  <si>
     <t>arian</t>
   </si>
   <si>
@@ -103,9 +88,6 @@
     <t>TlQAEKQQAAAKAU5GVBCaEAAACgFORlIlkBAZAAFoAfwB/AEAAP+OAQEfAAAAB9oiB2wtoBAuK4VtLQASFjWF1W0gFTwDiVZ6YBhBA5ba0iAORgh31t7AEUwIdNcJIRVQBI5hJsEPSwV0WJXBG0EFnuLOAQ9JBX7X+sEbQQOY25ZiFEoJevO1Qgw7DnfwuaIOMRB25LmCEDgOc3naohEyCnJ77eIMPAd5/QrDCCACaeM9wxNCDn3cTeMXTwuL+XHjDk8GeOeqIxdRC4LkusMbRA19BsVjCycFdevuYxwrBH2D8oMLIwR2/ALkEDwDgAFOpBNHBH8GUqQOMgF8gmXkESQGfIppJA0mBHT2beQbIA1qBaXkDTQGcvhFJRIoA2UGmAH///////8BAv8FBP8A////////Av8FBP//A/QIBtMFAB8B//8GAhT///////8IC5cBBfIHCSX/////AP8CBhMKCeIHBBL/Af8D/x8IC6gJBRMBAvP///8EBSEGCDwLCaILBRwG/6//////CvIICpsODWX///8EB1L/////E/MLCTsGCMIK/z8TEmMPDBMJBngNEBIXEXL///8JBkUOEhUUEGIM/x8JClYLDxESFEUN/x8JBmcNDhEHC6ETEmMUFzX/DPIJDWIPFCQXEWEUFzT///////8JEFH/E/MbGoUUDRUPCzP///8WFVIaEjMLCmMVGjQcF2MREDQPEjEWGCP/G/QaEhQLE3L///8YIRkbFSIL/78aGRH/////EfUQFGP///8fIfgbFRMW/x//F/EUEkUcHiP///8YHRMgHFIZFBQSFVEf//8hHWEaFCcVGEEdIRYgHiEZFyMaGyEcGhMVG1H/Ifb/IPL/GfMaHDEhIGL/////////If8bFf8Y//8h/0//////HvIcHSL/////////IPQdH28ABAAHAAQAAMQl6SqAGxYhcFw1oBEtNYVWSiASISKF2GFgFTsEimp+wAwaJXZWgiAYQgKZ2saADkUHeNTOIBJPCXfY+YAVUQWTZDJhD0kFdlihYRtEBaHhwoEPRQSB8NGhCA8VWtruIRxBBJjZiuIURwd/5K0iDzQPd+e14gwtD3fgtSIRJw5yfOICETIJc3fxQgw8BXr3BqMJIAJy4TVDFEANfttBQxhRCo33dWMPUAZ7/Y3jBxAEa+WioxdQC4PoqkMcQw2AA9HjCycEdvLe4xwsCICA6uMKIgV4+wJkET4EggBSJBRIBH4GWiQPMgJ+hGWkDCEEcI1tRBEbBnsGpYQONAR0AEHFEicDbbwB////CgWSA/9f////BP///////wP/Agf/Bv8fAf///wPzCAdSAAVTCgjCBwIT////////////AQbzCQxfCAMT////AP8vCg6YAgcTCQs2////BAE/AwgTCgvTCQYT/wLyBf8fCg6YCQczAgNSDP//BgcxCAo8CxA2DgsZCACZ////DRYkCg2cEQ9lDP//CQczCxD/FP//////BAn//////xbzDgtMCgArDf9PFhVjERAUCwiIDhExFxtGEAwfCwhVDxIRFxNh////DAv0DhYWFRIxEw8RCwhmEA8REQ4RFhVjFxQx/wz/EA8REhcTGxRRFxs1GP//////DBPx/xby/x71FxITEQ4z////GhlSFxUSDg1jGR40IBtiFBMzEhUxGx3/////////FBP/Ghw0/x/1HhUkDhaC////HCQpGRY1Df+fHiET/x3xGBT1EBdy/////x/yGRpCDf+/GBT2ExthICEz////HB8jIiAzGxcUFRlS////JCJhHhc3GRxSIiQWIyEhGxc2Hh8x/x3zFyBhI/8f////Gx4zGR9R/yT1IyARJP8/////IR0VICIh/////////yPzH/9v6xxpNmAPISOMWUXgETAMnNtaABUzBp9ZkWAYOAap2tYgDkkGhtbiwBFTCJTa+WAVUgasZB4hEEsDkehaYQkdGHVWsqEbNwSy4cohD04EmdjqIRw/BLF/igIIDwhs2ZaiFEsGm/G14ggdCHTmzoIOPRSO8dbiCzAOiNtBYxhQC6rhUgMUPQ+d9m0jD0gJlOWqQxdSDKXjvsMbRA6V7OajHC0JiwDuwws1A3r7AgQRPgWX/laEE0cFlASO5A4rCX0BOeUQKQZuUAH///////8BBigFBEEEABL/////AvMGBWL/A/QJBtMFARP///8GAhT///////8JDZcBBRIHCiUI/x//APECBhMJCsIHBBIAAUID/x8JDagHBTMBAmMIBBIABUEGCTwNCqIHChQM/1//////BPENBxwG/6////8LERQJC5sND3UMCCQEB1L/////EfMNCjsJ/x////8IClIQDiH///8L/z8REmMPDhQKBngQExYX/3//DPEICmMNEhQTF0YQDhIKBVgPExQX/38ODBIKBkX///8VFFITEjINC2MRFCP/GPQTDxQKDaMSGBQaF3P/EPQPDUP/FfL/GfQYEhMNEXL///8WGx8ZFCIR/1//////G/8ZFREL/68YGhP/////DvgTEjMWGRIa/z8XExQSFEH///8bGvIXGCIUFUL/G///////F/MYGTL/////////Gv8ZFv+0InpK4A4YJIjZSiAVLwadXE2AES8Mm1paYBsPIolxjoAMGihxa45ADRseeFmdABg3BazcwqAORwaI1NYAElIIl9Tp4AkOJWjZ8cAVUAavZSqhD0wDkeVSQQofF31WukEbOAO14cJhD00EmtneYRw/A6/sVeIJEw172YoCFUUGnvCpogkdC3rpxqIMNBGK5MYiDzsTjgD5YgoeBYSA+SIMOwmL2jWjGFAKq+FCQxQ8D50AVUMKEQSB9nWjD1AJluSewxdRDKXorkMcQA+W8uIDHSwJiwDmYwwzAn/6AoQRPQWa/VYEFEcFlQSepA8rB36YAf///////wIIJQcFIf8D9QYKQwgCE////wcAEv////8B8wgLIgYBFf////////8N+P////8A8QUHEwwJPwT/H/8A8QIHIgsJTwoCFgH/TwP/Hw0RlwIIEwsONgkE8wUAIgEKEw0O0wsHEwACUgQH/w4M/////////wb/Hw0RqAsIMwIBUwwJLwcIMQoNPQ4QPwsOJRD//////wkH8REOKgoDqP///w8XJA0PrBEUhhAM9QcLY/////8X8xEOTA0DKRET/xL//////wwO/w3/LxcYZBQQLw4KiBMWHxX//////xAO8xQYFRoWT/8S8QwOlREYJRoZTxMSEg4IaRYe/xn///8S/w4T/xUQ/xMU/xga/xn//////xwbUhoYEhEPYxcbJP8f9RoUFQ4RtBoe//////8S/xUU/xsfNCEecxkW/xQYQf8c8/8g9R8YJBEXgv///x3/LxsXNQ//n/////8g8hscQg//vx8hFP////8Z/xoYNB0gIyH/Xx4aFBgbUv////8h8h4fMxscU/////////8e9B8gUpgqaC1gEy43dWxCQA4kKXDpTkAaGCF3X1lgFhkCeuFpQBUzAnHReuAWHgN+VXpgGD4CgNvSIA5HDnPW4sARTQxk1wVBFUkEdGEeARBKCmhXkcEbQQaE49qBDkULc9j9QRw3BXrbmmIUKg9k2Z0CFSERZ/W5wgsxDGrvuYIQGxJm77lCEhESYfC9gg47DWvivUIUHA9idNrCES4MY3PaQhQdDGNx2mIPEwhpfO0CDToGb+sKAw4dCGvlPcMTPg1v3EkDGE0Ldfl1ww5HBGXpqkMXTAxu5cZjGz4JdYHlAwwkBXkCCSQNKwSBgyokECYCfgZKRA0yBoX/UkQTRwR/gW0EFCEDgfd1hBohC2EBeUQRHwJ9hIbEDiEDf/yWxBIaA34EocQMLgaA+AEB//////8CBP8JCP////////8ACPUH/y////8LBoEF/y////8EAB////8CBkMFCRIDBREJCDEHAE//////BvELCbEIBCID/x8JBRH///8C/x8LDpcACPIKDDX/////AfIECRMNDOIKBxIBAF8G/x8LDqgMCBMABfH///8HCDEJCzwODKIPCPwJAqj/////DfMLDpcTEFT///8HClL/////G/MPDPwJC9MND08bFHESEPMMCXgN//8bFv8UDv8MCf8TGBIf/5////8MCUUSFfEcF1ET/x8MDWYUFv8aFf8RDP8KDv8RFxEZGCIQ/x8MDVcN/z8bFmEVEh8MDoEXEREKEq8WGhMgGYESDPgUDRL/G/UaHCIYExEMEWEVGhQcGUH/EPIME2IZHBQf/38VGhMcHzb/GPETFyEbHTQjIYccERQVFjL///8eHVIcGiMWDVMdITYgH1T/GfMXGkH/HvIlI/QhGjQWG2L/////Jf8kHUIP////EPkcGkUgIiT///8hIhMp/38fGCgcHVIgHBYaHXMjJhMnIjEn/x8p/z//IPMcIYElJPEoJjIhHBcdHkIhIyEdHmQl//8oJiH///////8kHf8e//8o/x//J/EiIRMdI2L/IvEhJjEo/x//KfH///////8mIRQjJDL/////////IPciJzGYLVQ1QBQNO3ZbQsARJTt1XUUAECIxdlRKIBIbM3PZWaAVNwZ1VWkAFhsDd9JqABcdAn59dsALFx51VYJAGEABgtrCYA5HDnPV0iASTAtj1vmgFUsEeWIqoQ9KC2pXnWEbQwaG5crBDkYMddfxgRw1BnvnsSIPPhBq4bFCESQSZd+54hQ0EWXruUIMOAxrZdHCFhMLamjawhUTDWdt3qITHAlkdOZCETEIZnvtggw5BnD0/sIOHgdr4jVjFDsPcNpBYxhNCnf3dWMPSgVp5qLDF0sMb+W6wxs/C3WB4aMLIgZ8AQmEDSgEgwEmRAwZBX+BKqQPJwGCBFbEDTIFhv9WxBNGBICBbaQTJwOCAH2EERoDfYiKRA4mAYCBigQVFwN3AJpEExwDfoCaRBUWA3EFoUQNMgSBjNIEDw4GehwCAwH/////////BAr/CQIf////AAPxCwpjB///////AAH/Cgn/CQIfAf8fAATzCwpS/wbyBQsSCgMTAP//CgMkBP8f/wbxDQux////CAshCgUxAP///////wL/Cgl0E//PCwUTBv8v////DRKZAQoTDA42////BwJPBAsTDQ7DDAkTAgPyCP8fDRKYDAozAwVR////CQoxCw08EQ6TEgwcC/+f////DxQvDRKYEBNU////CQxj/////xvyFA78Df8vERcRHBlSE/8fDgpYDxZhFxwUEP8fDgtmDxQvFRoSFhERDg2BEBkSGP8f////CQ6UFRL/Cw//////Gxr/FhIRDA/iFBv0HRphFxERDBLBFRsVGhwiGRARERIRFhoTHB82////ExARGRwTH/9vFx0XHP8/GBMSEBEh/xvyKCKnHBcTFhUh////Hh1SHBoSFA/yHSQ3IB9D/xjzGRox/x7z/yT1IhpEFRti/////yj1JB0zFP//////GBxjICES////IiMTKyFRHxgXHBpFIiMS/////x/yHCBRIBwWGh10JCYjJyNCJicSK/8/ISAjHCKC/yjyJSYSIhwnHR5TIhwnJB4UKP8fKSYhKf8fLCcxIyITHSVh/yPyIiZB/yzzK/8fJSQSHR51/yrx/ynxKv8f/yzzJhwaJSghJSghHf9//////yzzLP8f/////yH0IycxKycTJikz////////</t>
   </si>
   <si>
-    <t>4298</t>
-  </si>
-  <si>
     <t>NURLELA PURBANI</t>
   </si>
   <si>
@@ -118,9 +100,6 @@
     <t>TlQAELgPAAAKAU5GVBCuDwAACgFORlIlpA8ZAAFoAfwB/AEAAP+yAQEfAAAAB/UlBwoVwBQoBZb0VuAMTQqTb80ADz4JogbagBA8DKHo6QAHQQWL7fbgCT4Dmob+ABQ7EJ0YVgETShOWl6KBFkEMnOWmoQdUApHq5gEKUwScsBHiHEEEpGImQgxHCpsoNSITPRWLYjoiCFQDnSJygg9IK4aidgIVOQ2a4s5CBVADnj7OYhFMFoZ50YIPNV6Gc/YCDyM/iTsCgxdGAqFRGgMQJBqJ6B5jCkMIoGcm4w1HEItOTgMQGCiL5WZDCFcHmuqiYwlTCpuWpqMQIDCD671jBVAIkwW+4w0+G3ypygMSPhOIttUDFEcJmPTmIwdNBpZ1/uMJTgSM9TrkBS0IjABJpAhGDoEGvAH/BvgDAXH///////8AAhUJBXP///////8FARX/APcDBxUMCaIGBxQKBVIC/x8A/38FBykJ/1//////AfECBxYKCXME/y//AfMDABj///8LCDMHBTMIDRYMBVYDBkP/C/UHABv/C/X/EPcNCmMDChMOEUb///8EBVMHDBMXDpH/CfMFAnb/////////FfgQCKUOCiMFB7UID1MTF1UfElQPCjUHCGYLELH///8JCkEMDyYXEYETFCMRDEMCB9gNFTUHCFYL/68VFiYSDUEMFxYa/2//////DvEWExIOD4ENEEQVH2EODIUPDSYSFiIUFxEXDBYTEhIVFpEcGDEgGVgSEGIL/4////8bGBEUExESFRggGTEYGSUiGnH/EfYOD4IXESkMFIEWGRIeGzEeFxUYFiEQFWgfHBEYHhUbHSH///8RF2Ee/y8iITEdERkaFyMYGTEVIIMf/x8eGxIbIRIj/0////8RGnEg/08kIjEbGCMZHBEZFRcg/y////8eHBEVC17/////JPYfGSMiJBQj/y//HfIaGzEhGhUbHjEf/y8kIyEk/x////////8hIiH///////8jIRQiHiMBBGjh4g4BBwB0IxD///8ABAAA6ycMGUAVKAeY+EpgDU0Lkm/VgA4+CKMJ2gAROQyh6d1gB0MFje324Ak+A5qE+oATOxCeZA7hBhoEjeQygQUYAYkYXoETShKWmJYhFkAMm+eaAQhRApTr3kEKVAWdrwHCHEEDqGMqQgxQCpsiQYITORSOY0bCB1YEn6JuwhQ5DpkodgIQSyqD4saCBVIDoHLJIg83hIhA3oIRSxCJa+bCDjFKimn+wg4zNIo9EsMXQQOj6xajCk0IoGIq4w8wIIpoMoMNTgmM6FqjCFgInHaWIxAeU4TqmqMJUwmb67XjBVEJlBW2Yw5AIXy0vsMRQxaIusWjE0oLl/TiowdPBpd2BmQJTgOP9TZEBi8IjQNJJAlHDn/UAf8G+AMBcf///////wACFQsFhP///////wX/HwEAVgMJFQ4LogYJFQwCYQH/bwD/fwIFMgsHUf////8B8QIJFwwLhAT/L/8B9AP/HwD/jw0JNA4Fkwj/H/8E8QUJKAsTWwcMGQv/X/////8E8QoPFg4FZwMGVP8N9QkAG/8N9f8P9hIMkwMMJBATV/8I9QcFVAkOJBYQsv8L9AUChv////////8Y+BEKpRALOAwCSgkSZBQZVhEVFBIOMQkKZg3/r////wsMUg4SNxkTkg8KFg3/rxgVNRIORBUUEhAOdAMK2Q8YNg4ZFxz/f////wgQshMOZRIPJRUiIxYbEhoWIxQSIRENXhghcRkQGg4UcRUiNBcbEhkQKxYUERUaMh0bQSIaWRURcw3/j////xcbIx4cQf8T9xASkxsZJBcVIhj/nx0gIhwZIw4XkRodIyAeQRsgJh4fMf///xMZcR4bIxoYKSIhMf8g8SD/PyQjQh8TGhwZNB4jEiX/T////xMccf///yQeIxkbdB0hERUYGCL/L/8m9CAdEREYNf////8k9CEaIyAkEv8l8/8f8hweQv8j8h4gQiL/TyYlISb/H////////yMkMf///////yUjFCQgI+0a+E6ADUgOrunhgAc/BabpjoEIUAO2k41BFjEPt+3agQpMBrys7gEdNwS+Y0bCB1QDuGRGAgtDCbYodsIPRTqp47oCBk8Dvj3aYhFGF6vtCcMKQAe4Xx7jD0ElqDwmwxc5ArVmQgMNTgqo6VbjCFcJueae4wlQCra9rqMWGweztrEjEjQZquq5AwZQCrYQwqMNSByft8kDFEYNtfPiAwhPCLJvBuQISgqo8TbkBi0JpgJNpAhFDJY4Af8D/wIBYf////////8I/gL/X/////8A8QME8wYJRv///wEAVgD///8F//8K/wgE/wMI9gcGMf8C8wH/n/////////8N+AgD3////wEEkQcIJgsJgQb/LwQAPgMI8wsPVQoLEgYHYwED7wUN1QcLFg//b/////8G8QwOEgcIUQMF/g0SYQwOQxAPQf8J9gcIUg4LFAcKYQUN6BIUERESFwoDbwX/j////w8LEwcIhQwSExQQMQ4UFRATIf///wkLYQwUEv8W8RP/Hw8OIQ3/H/////8V8xIKVAoNFxX/L/8X8xQMERAWEhj/T////wkPcf///xcQEg8OUwwSEQUR0/////8Z9hIMIxQXERj/L/8T8g8QMf8W8RAONBT/HxkYIRIZQf///////xMXQf///////xgWFBcUI5Qe/EYADkgPr+vVwAdABagUboEUPhK16oLBCFADuPDS4QpPB76u3qEcNgTCZFKCB1ADumNSwgo5B7YxgmIQQzqn465iBk0Dvm3Kog4XS6to3qIOJUKqPOqCEUMQrfT5QgswBrdpCkMOOCeouwrDGRQEsWImww8uKac6NuMXOAKz6UpDCVMJuWpKgww5CKvkjmMKTwq1v5pjFh4FtbyhwxErIKnsqYMGUAq3urGjE0cOtBi+Qw4zJpzz3kMITgiydRJECEUKqfcyhAcyCqUFSUQJQgyVaAH/AvoDAXH/////////AvgD/1//////APEPCDkEAyQA/6//BfYCBEQGCVf///8BAFcCCCcHBkL/A/QB/5////////8PEXoIAuf///8BBJIHCjkNCYIG/z8EAE4CCmYNElYMChMHBEcAAun/EfYHDRYS/3//////BvINBxYECJMPDLMLExMNBxcKCBMMGDQQDiEWEBILCDECBa4RGHEOEyMUEkEJBmgHClENCSkKCyEMEDIZE0EF/3////8VEVMMApITDiILDCIPFbcWGRIVGCUMCHYFD5P///8TGSYUFzH///8JDXESCSkNDjEQFiQZFEEQGRP/GvIX/x8SEzER/y//////GPMQDHUMERcY/x//GfETEEEUGhIb/z////8JEnEFFdP/////HfUWEBP///8bFCMTEEIWGBIZ/x8b/y//F/ISFEL/F/MaGSIYHUL/HPEd/x////////8aGzH///////8cGxIUFlTOJ/ROQA1JCXZxyUAPOQeGAdpgEDsLgufewAY2B3Pq/oAJPAKDhv7gEzsOgBZW4RJFEHvlpqEHUQN5mqrBFjwJhC3KIRYlC3/p6uEJUQR/qQrCFiYJhrEZ4hw+AodkHsIMOwp/JzEiEzoQd2M+IghSBH8hcsIPSSVqqIZCFTgKgz7KQhFJFHDhzkIFTgOCgtViDzBkbTv6ghcnA4Ni/sIOJThwP/0iGCwEh+QmQwpECYZaJuMPNxpzaC7DDT4LdFJZgxAYJ3XjZQMPESRx5WpDCFYGf+uiYwlRCoCSpoMQHjRt6r2jBU0IdgK+ww00F2WnxuMRNxJxts3jE0gIf/XmgwdLBn51AsQJSgJ3/0mkCEMQcdQB/wH1CgSz////////BAAV////BQIhDQeiBQYUCgRSAQAV////AAQSB/9f////////AQYWCgdz/wPy/wDzAv8f////DAgzBgQzCA4WDQRWAgVD////AgoTDxNG////AwRTBf8//wz1/wnxDgZhCw4VDQZBBQhR/wz2Bg0TFg+h/wfzBAF2Cf8fDP9/FRETDgZC/////////xH6Cwh1DwojBAa1CRBDFBhVFRI0EAo0BgllCxFB////BwpBDRAmGBOBEhQSEw1DAQbYDhEzCQtDDBevFRkmEg5BGRQSDxCBDhFEFSJhDRgWHf9v/////w/xDw2FEBIiFRmRFhgRIxtfEhFiC/8fF///GA8ZDRRhEhkhHBrxIxv/FRH/DP//////FhoSIR1h/xP2DxCCHhoRFhIRERdvGxz/GBMpDRaBGRwfIR4xIRz/GRT/FRf/Ih//GyL/HyH/Hhj/Ghn/GiEVHiAh////ExhhIf8vJSQxIB0SGBoxHBv/FSODIv8fJSEhHiQS////////Ex1xIv8f/yXxHhojHB/xGxX3I/8v////IR8RFRdf/////yb2IhsvJSYU/////yDyHR4xJB0VHiExIv8vJv8v/////////yT0JSEj9CT6RsANTAl5cdHgDjwHiefWQAc4BnUE2sAQOwqC7fbACTwChYX6YBM6DoIXWkETSA995prhB1EDfJeaYRY/CYQu0kEWJQuB6d5BClIFg6L+YRYlCoSwCcIcPwKLYypCDE4JgyY1QhM7EHliSsIHUgSBJ3ZCEEgiaKN6AhU3C4V2xUIPM1ds4cqCBVADhEHaghFID3Nt6sIOL1Fvag5DDi8ccucaowpLCYZoNmMNSwd20VlDDxErcuhaowhZB4F1kiMQHFNv65rDCVMJguu1AwZNCXgMukMORxpnsLrDEUIVcri9oxNJCYD23uMHTgeAdQpECUwCewNJRAlCEG+wAf8B9QcEhP///////wT/HwD/XwMGFQ0HogEEQwf/b////////wUGFQoEYwEAFv///wEGFwoHhP8C8/8A9AP/H////wwGNA0EkwgOFg0EZwMFVP8M9QMKJA8TV////wIEZAb/H/8M9f8J8g4KYwsOFQ0GUgj/Lwz/bwYNJBUPsv8H9AQBhgn/H/8M9/8R9A4KRf////////8R+gsIdQ8HNwoGRg4QFBIXVh8UVBAKNAYJZQsRQf///wIKog0SOBcTkhQSEhMNZAMJ2A7/Pw4LFAz/r/8U9RANQw8NhRAOJRQfIhUXEQ0XFxr/f/////8P8hkV8xIQIQ4RRf8f8RcPGg0ScRQgNBkW8RcPKw0VgRQfNBkY8RYYIyMaof8T9w8QkxoXIw0WkRQZPx4cQRT//xse/yIc/xgV/xgeJhwdMf///xMXcRwZLxURRyAfMf8e8R7/PyIhQh0aExcYQRwhEv///////xMacf///yMcMxcYdBsfERQMHiD/L/8j9B4bEREMPv////8i9B8ZLx4iEv////8d8hocQv8h8hweQiD/TyP/L/////////8i8hweYw==</t>
   </si>
   <si>
-    <t>13424</t>
-  </si>
-  <si>
     <t>ANGGIA AYU PUJI PRIBADI</t>
   </si>
   <si>
@@ -130,9 +109,6 @@
     <t>TlQAEEYKAAAKAU5GVBA8CgAACgFORlIlMgoZAAFoAfwB/AEAAP+qAQEfAAAAB/8WB2J2YAk7B5Px1gALTg2XdNqgD00Mld7+AAQiBo5gLeEMPg+h4YKBCkAHoHmqYRJCFJrsGsINRhChUEECDz8Ym4aCYhQ/E5NVkqISLm6OSdpCCVMGqEXaQgxVBqg5/YITQRScTSpjBlQEo89SQwRLA5WzfsMYSQOFQqojClcHnTDGoxZQB4VFGSQGTQmYrppEFjkPei7uRAgyBo4GCAED/x//////AvUBDjkCBBQF/08DAEP///8B/x//////BvYHBIIABRgHD+j/////////A/gB/08CBiUHBXH/BvQHC2T/A/gABHEFBEX/////CfUKB3H/CPIMCxL/BfYEBnEM/x8HBCoGCUIKFEcIBiX/////EPENCjEMC1gIBkf/CfEQDSUO/y//BfQHDCMSEeIRCxP/BfcIChUNFJj/EfsMCpQJ/z//EPQP/x//BfILDCYRE1IODR4RE3T/////A/j///////8UElIMDdQVEyQOC1IMDRsS/98UFS4RDdIJEBL/////////D/QRDU4UFeIS/y////////8VEdr///////8TEi4U/98BBEmhQhIABwAEAAD/GGF+IAk7BpX1ymALTA6XcNogD04Nl+D2QAQjBpFcOWEMPw2i33bBCj8HoHOm4RFKFJzwDiIORBOgTknCDkAVnX92AhQ2F5NNkiISLm6PRMriEigplDzSYhMZIZZK4kIJVgapRupCDFUFqToNoxNHEJ1MOiMGVASiz0KDBE0Cl7VygxhKAohAugMKWgedMdYDF08HhUYlRAZMCZewiuQVPA58MvZkCDEFkCABA/8f/////wL2ARBKAgYpBP9PAwBU////AQAm/////wb3BwSSAAUZCP/v////////BQMYAf9PAgYlBw54/wb1Bw11/wP5AASBBQRV/////xL1CQdi/wr2CA0j/wX3BAZyDv8fBQeSBglCChZHCAYm/////xLyCwoyEw6GCAZI/wnyDAsiEw6oCApiCf8/DA8RFxPrCwoSCf8//w/xEP8//wX1CA5EFBPjEw0k/wX4CAoWDxaZ/xP7DguRDP8fEhRC/xHy/wP7DQ43ExViDRBCExWE/////wP5////////FBU+Dg/kFxU0ERCGDg8rFP/vFhc+Ew/iCRIj/////////xDyEw9OFhfiFP8/////////FxPr////////FRQuFv/v1RZhgsAINwew9tJgC0wQu23eIA9KD75sqsERRxrH8wUCDjsXv0xi4g9CKrd8bSIULyG1TInCETNgsS+SghIcY7BBzSISLSCyN+kiFCcSuUvuQglRBss8+mITPxa2RAoDDEwGwM86gwRMAbhNQiMGUQO/s3ajGEkDqUC+IwpVCMUv1uMWTgemRCkkBkgKwa+Z5BYwEZ8wDqUILQeuCAH/////////AfMDDrcCAxgL/5//APP///8BABX///////8DC2b/AfgC/2////8GBFH/BfQNCyP/AP0CA4EN/y8EAkwDBlEHFCYFAxX/////EPIJCEINC1gFAyf/CPEKCTIJDRYHBRIDBnL/CvEVDbf/B/II/x8KDCEUDBEJCCEG/z//EPMPDiP/AfgFB1gNETIVEckNCYEGCjEQEkIRDxYLATwFCSgS/68LDzERE3T/////AfT/DvH/AfYLDSYRE1L///////8UElINCsMVEyQOD3UNCRgS/98UFS4RDNIKEBL/////////D/IRDE4UFeIS/y////////8VEev///////8TEi4U/++TGV+OgAg5B7H6wuALShG65NYABSIGrWnigA5GD79fBmEDDQqsZ6oBETYayPr1gQ4zGcCAYcITKye1Sm6iD0AjuESWYhIQYrArlqISHFmwSZlCETE4skPdYhIuG7M38SIUIhG6Sf7iCFEGyzsOYxM/ErdEFgMMQwXAzybjBEYBvEtS4wVOAr2zZoMYSAKtP84jClUHxS7mQxdMB6VEOSQGSArAs41kFi4QoDQaxQgoB7AsAQL/H/////8B9AUOzAMFKQ4ElQD/T////wAGHggE4f///////wIBYv///////wUOd////////wIGHg7/3/8A/AP/f////wcGUQcINBARNQQB6gMFgQYFNf////8N8goLIRAROQIG5AUHYQsXJhQLkQgGVgcKMRMMQQwQGAkIFgUHgv8T8xAOWAgGJQcJEQ0MIRQQlwQJ4Qr/Hw0PERcPEQwKEQf/L/8T8xIRNP8E/QgLaBAUQxgU6xAMkQcNMRMVUxQSJw4BTAgLNRP/7wgOlBIWJP////8E+f///xEEKw4QNxQWYv///////xUWPhAN4xgWNBIOYxAPKxX/7xcYLhQP4xP/P/////////8S8hQPThcY4hX/L////////xQQuf////8W8hQXPv///+8U7tYgC0oNenXaoA9LC3sJ8UAQHQl9hf7AERwIeWEp4Qw9DIXhgoEKPQaCfKphEj0ReOgawg07DINROqIOQRJ/kYZiFCsRe0rKYglWBohG0kIMSwaFOgGjE0QTgU0qYwZUBYfOTmMETAR7tHKjGEgDbUKuIwpWB3wwxqMWTAd1Rx1EBkoKfa2mRBY2EGPwAAEEFAX/T////////wD/H/////8C/wcEggMG/wUE/wH//////wL///////8G9QcEcf///wD/TwEGJQcFcQIG9AcKZP////8E8QQDVf////8J9QsHUf8I8RELsf///wUGYQv/HwcEGQYJMgwQgwcGNf///w8MExAIkg3/L/8F9AgLMxEQ4hAKE/8F9wgJFQwTmP8Q+wsImAn/Pw8RQg7/H/8F8goLJhASUg0MHhASdP////8A9P///////xMRUgsM1P8S9A4NdQsMGxH/3xP/LxAM0gkPEv////////8O9BAMThP/7xH/L////////xIQ6v8VY34gCTkGf/TKYAtLDnt02iAPTQx+XTWhDD4Lht52wQo9BoR3puERSRB67BICDkUPg1FGYg5HD4GJeiIUPhN7TqFCEjFpeEbJghIuKXtK2kIJVQaKRt5CDFUFhjoJoxNJEYFNNkMGVQWHz0KDBE4EfbVeQxhKAnNAugMKVwd9M9LjFkoHdUYpJAZJCnyuliQWOA9l/AD/////////AfQDDnoCAyQE/1//APT///8B/y//////BfcGA5IE/x8B/08CBSUGDHgDBRUGC3X///8AAYUEA1X/////CPYJBvL/Cf8HCyP/BPcDBXIM/x8EBoIFCEMJEfMHBTb/////DfMJDPcRDP8HBf8I//8QCv8RDP8HCf8I//8QDf8O/z//BPUHDEQQEeMRCyT/BPgHCh8NFJn/EfsMCp8I/z8QEkL/D/L/AfcLDDcRE2ILDkIRE4T/////AfX///////8SEz4MDeT/E/QPDoYMDSsS/+8U/z8RDeIQ/z//////////D/QRDU4U/+8S/z////////8TEes=</t>
   </si>
   <si>
-    <t>4014</t>
-  </si>
-  <si>
     <t>SRI HARYANTI</t>
   </si>
   <si>
@@ -145,9 +121,6 @@
     <t>TlQAEFwQAAAKAU5GVBBSEAAACgFORlIlSBAZAAFoAfwB/AEAAP+nAQEfAAAAB/8kB3wKoA4mBIhrMSAMRAqOcWYgEVAIhuyZAApPCYVdwkAHMgd/i9bAGlIJi3T5oBJCCIf0FgEPUwmGABYBEzYJhlpGAQdRAZNkfUEPTgqGf5bhFlYLiloFIgtXBZjnCQIOVAiTYh7CEkYNjQIdIhVUEItgJaIQSQuYlJniG1MIh36qghhTEpFcsWISUQ6b4snCD1AFpHb2IhhCG5LyBqMTSRSREiYjF0okkFBhAwdLBZo9ZgMXKmWKRmlDElMQjCCGgxg+FI1KkgMMVwijKZZDFzsgijuaAxRUEYmlooMdQhOSn0EkG0MShBFGxBhFEoEWekQYSA5/JwGFDkMIiQawAf///////wUCUwcBgf///////wACEwcDggEAM////wULKQYJUgIHFgwJogT/H/8B8v///////wMHFgwJogL/L/////8R/AsIYgcCFf///wUIIQ4KgwYOGAr/PwQDZgL/T/8L8w4KcgcGEf8F8v////8E8gcKRwwYi/8J9wcIMgULUhANYwoIIwX/b/8S+A8OQ////wkHhAoNExQYkw4QMxQcdgwJOgcKYxANEwoLYw8SFBYTZBESJBMOQQ0ISAv/T/8N8woIZw4SFhMUZA8FLP////8b+BUSQhMPFAUR4v8f8hUWIRQMKxAOZP8X9hYaNBMWJRocYRj/fw0QdBYPFxIRJP8f8RkXQRcZJBocFRgTsw4SYRsZIh4WIhMSZBX/H/////8M8xQcdiP/nyMeohoWRBf/LxsdESMcVv8U9hYZFB4iJCEiNB0ZERcSJv8f8////xgMaBQaFiEjsyEjGx4aNRkRGRsgESP/fxwaghYZIh0hMhH/T/////8g9h0bUxsfJv///////yEeE/8i8SMYrh4dIR8gcf///yMYnh4hESD/P////////xweNyL/nwEEI2XDFgAHAAQAAP8nfQ5ADiYEiWo5oAtDCo5xbqAQTweJ741gClEIiF7G4AYxBoGKzkAaUgiLeAFBEkMIiPgOgQ9VCIgBFqETNgmGWU7BBlEBlmOJwQ5WCIl8kmEWVguK6v1hDloHk1kRwgpWBZsIFcIVVg+OYCZiEkYNkF8tYhBLCpuQjYIbVQeLe6oCGFUTk+a94g9OBaVavQISVAudc/KiF08alff6AhRNFZQYIqMXSyKRTXHDBkkGmidyQxctT4tFdSMSVRCNNHajFihZiR+O4xhEDY6kmkMdRxKTSp7jC1cHpCeiYxc5GIs4quMTVQ6KotGDHSUgip3qQx0lIIelNWQaPBSFDFYkGUUSgxSChBhJDoEkCaUOQgiL1AH///////8FAmQKAbH///////8AAhMHA4EBADT///8FCDcGCVICBxYMBLH/////AfH///////8DBxcNCaMC/z//////EfwLCHMHAhX///8ICxQMCkIGDxkKCTUEA3YC/1//C/QPCoIGAhf/BfP/////BPMHClcNGIv/CfcDB4MIDiYQDFIKCCQF/3//EvkOD0QOEDITGGINCSoKBiT///8JB4QKDBITGIIREhQUDzEKC2QF/68QDBMKC2QOEhUWFHQYDCIKCFcPEhYUE1MOBRz/////HPgVEkIUDhQFEeL/HfMVFjIUFhUaHlEYDWgQDzIeEyEQD1T/FfQWGjMWDxgSETT/HfEXGiIVGxUaHhYTFFMOEmIcGTMgFjMOFZIR/1//////CfsTHmYm/48fJhsbFhUXETj/HPEmHkb/FPMWGxQgJSQlICMaFkUXETgZHxEjJSUfGSEXETj/HfQR/0////8hI/YcGUT///8YDWgTGhYkJsIjJhsgGkUZERkcIS8m/38eGpIWGzMfJEMd////////Iv8mHP8XIS////////8jHDEcIiP/////JfMkIBP///8lJiogHzIj/x////8mGJ4gJCIj/z////////8eICcl/5/rIGomwAs6BqtkaoAQSQqp7plAClAJpF3S4AYyB5SJ0kAaUAit+hJhD1MLqXgS4RI3C6h6GuESHguoXFqhBk8CtWGFwQ5SC616lqEWUg2x7P1BDlcJtVgR4gpWBboHHaIVUxK2j5WiG1IKrHSqAhhRFbjmtuIPRAi9WL0CElAQufrtwhNFGLRp+mIXQCK1HCLjF0orryBZAxcjZ6tReeMGRQe5RHkjElQUtJ+aYx1CD6pHouMLVAnHNrIDFFMSryK9Qxc7FaWiPQQbORadEEbkGEQWmBGChBhFE5ssDcUOPAqhgAH/////////AfMFAnICABP/////BPIGBVQBBRULA7H/////APL///////8CBRUMCKIB/y//////DvwKBmIGDRkJCDQCAFcBBEEFARX/BPL/CvQHCRIFARUGBBP/CvMLCUL/////A/IFCUcMFov/CPcCBYMHCiIQC5MJByME/2//D/gNC0ENEUkQFmIMCDoJBzT///8IBYQJCxMQFoMODyQRC0QJB3gK/08NBCz/////GPQTD0IRDRQK/48OGCITEiEPESIXGWEWDGgLDWEZECILCpcNE0QSFzQTFR8XGSUQEVMND2ESERQND3L/GPEUFxEcFV8aEiMTDxMOGFEbH/8aEf8SFP//GP//////DPMQGWYf/58fGVb/EfQSFS8aHiQO/0//////HPYbFGH///8WDGgQFxYdH7Mf/38ZF4ISFT8bHTIdHxv/GvMVFPQY/28bGBb///////8dGhP/HvEfGasaGyEYHHH///8f/58aHREc/z//////FvkZHToe/5/KInQqYAsyB6tvbkAQTgmr8YnACk8IqIbGABpQCK5m3mAGLAaW/AYhEFEKqWZiYQZLAbdhkYEOUwqudpLhFU4Mse71oQ5YCbQMGUIWUhG3Vx2CClEFu1w+YhE0DbZcRiIQLgu4jIlCG1EKr+qmQhBCCrxvqmIXTBa6V82CEUsNuvvtIhRAGbVk+sIWKx62HiZjGEUjrzhqwxYoaqtOhYMGQQe4QInjEVUTtZyKAx0wDasZnmMZQAqoRbKDC1IIxyXBgxc/FKSfwQMdLRKnNMoDFFMPr6U1RBo6F50MTgQZRReZD47kGEUTnSEdJQ89C6GYAf///////wEFSQIEIgIAFP///wMIKQUGQgEFFgkEsf///wD/LwH/L/////8O/AgFcv////8A8gIHGQb/PwgMWQcGNQIAaQEDQv///wQCMgUHVwv/j/8G9wIFgwgKJgkLIQcFJf8D9/8O9goMRAoNMw8WYgsGKgcDJw4QFBIMUQcIZAP/r////wYCiQkNJQ8Wgg0LFQkBPQoQFRIPYhYLNQkFOQwQFhEPUwoDHP////8Y9BMQQhARMhcaYv8L+A0MMhEMFQr/Tw4YIxMSMRr/Lw8MJAoSMhUXcxMVFRcaFREMJgoQURoSYQoQcw4UQhUXUhkVNBcSMxMOJf8Y8SEdoxcSRRMURBkbIf////8G+wsaJiH/jyEaRhYRsxIVFB0gJA7/T/////8c/xkUQR4fJBsVIhQOOP8Y9P///xYLaBEXJh8hwh4hGh0XNBUUJBn/LxQY//////8e/yEZ/yH/fxoXkhIVMxsfMxscH/////8g8x8dE/8g8iH/rx0bMR7/H////yH/nx0fIh7/P////////xodJyD/n/8lbTXgC0ALc3BqwBBOCG/smSAKTgpt/KkAEiYJbnLCQBEpCHON1qAaUglzdPmAEkEHb/UOYQ9RCG/9KUETNApsWUrhBlEDeWSBAQ9VCWx+koEWVApy5gVCDlYHdloJIgtWBX4CGWIVUw5xYSJiEkUMc2AlohBIC4CTlcIbUgZwf6pCGE8Qdl21QhJRC3/gzaIPUAWIe/oiGDkVeO8GwxNCEXcPJkMXSRt3Ul1DB0wGgiFqIxcrXXBIbUMSUA5xTYZDDFMGhSGKoxhBEHOnooMdQRV8Oa7jE1QMcCmtAxdAEnSb9qMdIjxwkUEEGx0ScBBSBBlEE3AZdiQYRgxvJwWlDkMHeLwB/////////wHzBwJyAP8/////BQMiBAkhAQcVDQmi/////wDyBQYTCgRhAAFS////AgA1AQMhBQYSCgdRAf8v/////xH8CwhjBwQSA/8/BQgiDwqDBgsUCg00CQJFAQRB/wvzDwpyBwYi/wXz/////wLyBwpHDRiL/wn3AgeDCA4nEAxjCggjBf9v/xL4Dg9DDhBDFBt2DQk6Agqz////CQeECgwTFBiTERIkEw9BDAhIC/9PEAwTCgtjDhIUFhNk/wzzCghnDxIWExRkDgUs/////xz4FRJCDw5EBRHi/xz2FRYhFA0rEA9kERIxFho0ExYlGhthGP9/DBB0Fg4XEhEk/x3xFxoSFxkkHhohGBOzDxJhHRkSHhYiExJkFf8f/////w3zFBt2JP+fIh8hHhYkExeC/xzxJBtW/xT2FhkUHv8v/xj2/w34FBoWIySjISP0HxkhFxEo/x3zEf9P////ICEfHxxjJP9/GxqCFhkiHyIyIiQbHho1GRwSHSFvFx0R////////IRzxHxX/IP//////IyL/////I/8fHh8hICFP////JBuaHh8SIv8f////////Gx43I/+f/yZrPWALQAp1cHJAEE4Gc+6JoApPCHL/oaASJwhscMbAECkGdorKIBpSCXN6AQESQgVx+grhD1IHcgAlwRMzCW1ZVqEGUQN9Y4mhDlMHb3yS4RVVCXLp9cEOWQZ4CBXiFVYNdFkZogpTBIRfKgISUA14XzFCEEoLhJGJYhtTBnN7psIXUQ94XL0CElUKgePB4g9RBYp28qIXQxJ89foiFEwRehYiwxdLG3hOaeMGSweDJ3qDFzg1cUSB4xFVDXNKkuMLVgaHIZIDGUQKdKWWQx1IEX0nuUMXOw91N77jE1QKcqPNQx0lInmc6kMdJSl0ozlkGjoYcQteZBlGEnIYgoQYRwxxJBHlDkMHfMgB/////////wHzCgKhAP8/////BQMyBAkyAQcWDAmy////AP8fBQgTBgQhAf8v////AgBGAQMxBQYSBwkjAf8//////xH8CwhzBwQSAwUiCAsVDApCBg8ZCgk1/wL2BAMi/wvzDAoxBgMT/wXz/////wLyBwpXDhiL/wn3AgeDCA0WDA4hCggjBf9//xL5DQ9EDRAyFBtmDgkqCgYkERIUEw8xCgtkBf+v////CQeEDBAkFBiCEAwTCgtkDRIVFhN0GA4kDAgmDxIWExRTDQUc/////xz4FRJCDw1UBRHi/xz3FRYyGxQhEA9UEhUUFhozExYVGhtRGA5oDBBjFg8YEhE0/xz1FxoiFRkVGhsWFBNTDRJiHBkzHxYzDxWiEf9f/////wn7FBtmJf+PHiUbHxZFFxE4HRxBJRtG/xPzFhkVHyQk////GA5oFBoWJCWyIiT1HhkhFxE4/x30Ef9P////ICL/HBlEIyUaHxo0GREZHCIvJf9/GxqSFhk0HiMzHf///////yH/Hxz/FyAv////////IhzxHiH//////yP/JR//////JCUqHx4xIv//////JRubHx4jI/8v////////Gx8nJP+f</t>
   </si>
   <si>
-    <t>4015</t>
-  </si>
-  <si>
     <t>Frisilia</t>
   </si>
   <si>
@@ -157,9 +130,6 @@
     <t>TlQAEPIUAAAKAU5GVBDoFAAACgFORlIl3hQZAAFoAfwB/AEAAOOQAQEfAAAAB4AwBxY+IBQQB3KWhcAWEwpxkqVgAwgDhY2mQBYXDHeHwWAUHwh7jN6gBS0HeQj1QBAzC3EL9WAUJAp7i1lBGh0JdAhygRckA3qVduEKQAxxEXaBHQUOb46BQRwYFnSMpSEFQAh/C7KBDjMJfQy24QdDDHuJusELMgh5DcLBHQYGeRPugQo+DXwQ9eETGwp8DvahHBUIeREVIg0oBoGSLiIPHAWCGTnCERQFfhBJwhwSB4CXTqILHAN4jHGiGigGeomOwhMiCX4IlgISIAp/C5oiHBQIfw6pwhRDCn4WxkIRNw57hWpDGS4FfAN2wxcnBX0TrYMZQA56mMFjEE0EhZTVowRBCY8X2QMSPgOFkR2kBUMKiZcphBdCD4MGTiQZIwmFDHEkGgwLihZ+JBY3DIaYrcQUNwWGlvoEDS4Vho0F5QocGYKLHsUOHhaBjR6FEB4RhAZAAgEEEwYCX////////wD/H////wgDQQQFN/////8G/wUN/////wD/HwH/HwgJNAcEIf8A8wEDMQgHMg4GcgL///8G8woNFf///wkTJQ4FYwL//wAHUQkTJw4GUf8E8gP/LwcBFP///wwUFBMJYRQaJRMOQwcEJP8I8QX/HwYOQRASEw8NI/8R8RMMUQP/L////wj/H/8L8REUIxsJgf8F9QAPwRIkHv///xcW8hUQMQr/HwYJUxIkHv8N8f8F9AoQIQUKMQYOURYVEhIPEf8Y9BQTEwwLIf///xkkHv8N8Q8KExAVERobExcW9QYHVwkUQv8Y8hoTMgkMIxH/HxwjGBn/LxIGGQ4WMRAOEgkXfxwjGCQV4Rsc/yQW/w4G/xMa//8d8hoeJAkUQv///xIQExUXLx8kHv///xMMFhj/Lx0gFiEecxcT8wkach4hFB8cIR4jGB//HxYXHxMbQf8o+yAeUhoYEv///yAhNCMckRsTFBQaYyEjFiT/7xYcIRseIh8eEx3/X/8i8ichUSInFColhR8eFB0gYf8o9CclRSEgEv///xkfZiElUSosKiYkmP8S/hkj6Cb/L////yosKi0j8RkfZiEnUSQZLh8j6S3//////x8iVP///ygqFCslUSn///8q8iciFB3/v////y8q/ygi/////////ysmJyUnJSgpLyUiSCr/L////y8mVSYlKisvYS7/H/8t/yYZ/yMs/////////ywjGisvYf////8t/ywlGSv/X/////8u8QAEAAcABAAAfzIcTqAUEQZ0m3VgFhMIc4+iwBUdDXmKwaATFQl6kdKAChkDdZHWAAUtB30R6uAKEAVzCv3gEDMMcgv9ABUeDHsQNUEUIAR4kEnBFSkDeItJwRkeB3SWckEKQQ1yCHIBGCUCe4Z9oRsYFHaNmaEEPwqBibIhCzMIeQu+AQ8zCIIJwmEIRA19EvYBCz0MfA8BYhQdCnoHAiIdFAV8FhGCDxUIhQ8Zgg0oBoKJIsIOJgaDlT5CCx8GeZZJghIWBn0UUUIdEQmGi2UCGikHepSKIhMjCX8EnqIcEwiBBaKCEiALgA2xQhVDC38WzsIROA57j2KDGCsFfgt+QxgnB32ZueMPTQSIErkDGj8LeZLJYwRBCJEW5YMSPQSHkxVEBUMLipcdBBdEDIOYKYQZJBCBCVakGSEKhxOKhBY1C4WYpUQUNQWJjO4kCRoUkpbypAwwE4aFEiUOHhWElxLFDyAQhlgCAgMjBP9v/////wHx////////CwIxAwAh/wDyAf8fCwgyAwYU////AQIhCAkfBwYS////AAdhBgwTDwVi/////wTyDA8l////EQwzDwViBP8fAAdhCRb/EQZB////AwgRDQovCQfxAwISAf8vChT/EQb/BwP/CAv/CQj//wv/DRT/ERD/CAET////DhwWDQofBQYjBxFBEBMkEg8zFRw1FBFECgL1Cw4RCwET/////xXzHA1R/wX1BgxjEiYe////BQxCBxFSFxMiJhLhGhb/FxAyDP8fBwpPEyQYJv/vDwUVDBAxHxki/w/xEhASERcxHB0TGhb/EQofDRVC/xvyHBQyDQ4z////GiT/GBf/EBH/CRT/HyQXGf8vEwYVERgxExETFhT0GiHzJhfhEhMiFxgjISgeJv/vFgr/FBz/HR//Jhj//x7yIBxBDRVC////FA4VFRsxHiIWJyCyFhr/DRyCICQZHxkS////IiBiHA4XG/8vICcYISYuGBovHRwSIiM0JB+BHRQTFRxiIiQWJv/vGB8yHSAyIBw2Hv9vJSMhJyRVJSkULSeVISAkIv8fGSFmIydRLS86KCaH/yr/KSc0Ix4X/////xP+GSTnLihh////LTE5LyShGCGGIylRJhkeISToLv9P////ISNUJSo/KywTLScxIyX//////yv/LCn//////yzzKSofHv/P////LS8pJykjK/8/JykzLP8v////MS5YKCZGJC/C////////KCQqLTFhMP8f/y7yLxkeJzGh////////KCcZLf9f/////zDxtBiQvUAVHgaBBeLAECoFh4zxYAU2BpiUfkELQgeGjKUBBUAGm5KqQRwaCX4MtgEIQgaXirpBCzIIjA66oQ8yBoOMyUEbFQWDFuqBCkAGkpY94gsiA4+OcSIaKgaHD3kiFTsKkhW1whEsBpASrYMZQQeTl71DEE4Cp5HNQwRBCKkXzmMSNwOkkhlkBUUKqpYlZBdCBZ0TkeQVMQafmbYEFDEEoY8NBQ0nFI8gAf///////wUNTQgBYgkNOAgGR/////8A8v////8B9AMEFf///wL/HwEIQQ4HQQYEI/8C9f8G8QoRLv///wD/T/////8M9AkIEwoRHv8E8f8C9AEHcQIDMQEIUQ4LMwoGEQ0OJAsHQQMBFAAJYgD/bwX/H/8M9A0IYgsRHv8E8QYHEQgNIQoHEwgNQw4THhH/7wgJFP////8P+BINsv8P9g4LMwgBKAkMUg8QNxH/7wsIFA0MNv///xQSRA0MaP///wsOdwwSwRYXSxMRmP8K/gsQ6BP/L////xUWNP8Q8QsOZgwUsRELLg4Q6Rf/P////w4PZP////8V9BYSUf///xYTJxIUNA//fxIPSBX/L////xcTZBMQOxIWtv///////3Unj6mAFCQHf43WIBIPA4iI5eAENQWaC+ogFRoEiAvyYBErBYgONQEUIwOJjknBFSsBjoxJIRkjBIsXaQEZGQKNlHKBCkMIiZSWoRsbCYOSncEEPwebj7KBCjMKjwvCgQhECJgPwkEQMQaEi8GhGhUEiBLZIRoNBImP6SEZDgOMFvoBCz4FkRAOIhQbCosPGSITFwiIli1CCyMEkY1hghkrBokQgaIVPAqTE8UiEi0Gk5ixww9NAqgSuQMaQAeTkL3DAz0IqRPWgxI1AqWUFeQERAuqlRnEFkIDnxOdZBYtBp+ZpoQTLAOkk+mkCRkPnpb9ZAwrEZSQBcUJGRWTlxpFECIUk44mxQ4gGYuVJgUTCxWU1AH///////8HA/EBAhX///8AAxEFDvYEAhT/////BPQJCxT///8HBv8FAfH/APH///8FDvUJAlT///8BAxEGE/8OCf8BAP8DB/8FA///B/8RE/8OCf8D//////8KCP8TBv8PEf8TBv8DB///Cv8C/x8EDlEUDPINCzMI////////FvYPBh//AvQEDYESGx7///8CCTIEDmIUEvIbDeESGRgb/+8LAhQJDDEUGPQVEkMJBBUFEf8IB/8K/x//FvMQE/P/Fv8RE/8GCP8P//8GCP8Q////Fv8XE/8YFRH/C/ENDBIOFD8WFxIbFO8OBh8IEf8XGP8bFf8OBf8GE/8NEhEOFE8YHR4b/+8TER8K/1//GvccF7EaHFkYFSIUE/IRFvEaGSYb/+8VFB8X/y8VGGYWHLEgIkodG4f///8eHDQXFlf/////Df4VGechHfH///8eIBUiGbEVGGYWGrQbFR4YGegh//////8YF1ga/z//H/MgHFH///8mIFIcHjMa/28ZHEUeH1L/JvQkHVQdFf8ZIv//I/////8dGSogJWH/////I/8dIf8ZIv////////8dHBogJlH/////JfEiGRogJGH/////I/8dIBQf/1//////JPF1OYfF4AUwCWuJxaAPFApoislACRANb4vaYAsQA2cK4iAHFQNtB+bgDBIIawbqABkTDHIG9cAPMw11DvnACQwNdRAJwQ0WC3QHFaESFQp/ET7BDhYCeoxRYRYjBW4EWSEYGgRvEmahDRQCcI96ARMSB3qShuELNglzj6lBBTwKbI2p4RESBoONsmEOGAp/DrbBBzsPZgjJQQ4iBoML4cEPHg6DCerBCzkLgYrqYQ4fCIUTAcIRGg98GA7CDhsMhxURwgwlC4WTIuITCQVymV6CERsMgZdeIhQVEXeNeUIUIAx1j5JCERUIdQmpghEeEW4LqcIUOwx0BK3CFxgJdImxgg4KDXMMteIMFQtzFMpCETYXaI1ZgxYXCm6KamMZLQlsi2oDHBoHbA2JIxUcDmkKiQMbGQdtComjFyARahOtYxk4EWeWvUMQRgVrltWjBDwJehjdQxI4BWySHYQFPAlxmCmEFzsYdJA5hBogC26MSoQXFQh5CV3EFRQRfwZhRBkgC3UWgiQWLxd/mLHEFDEJeKwC/////wLxBBEW/////////wbxCgcyCQUx/////wHyAwgfEQRxAv8f/wXxCQ4SFAhvCBT0Ef9fAP8f/wLxCQsREAg/A/8f/wHx/yP8DQoy////////ChIWCwkyBQES/wbxEBT/EQT/AAL/AwX/Cw4SEAg/Bf8fAQcyDA8TEwtzB/8f/wbyDxMTDgQRCQcT/wrzCv8fBg0x/x73Eg9C/yP5HA9iDP8fBv8/FhMxEBEVAwkiCw8RCwoTBgxSIxmPEhMjCAXzDhIRExcT/xTy/wT1CBTxGy9O////CwomDw0kHBk/FhMxEA4RChJxFhUhFxQhFy8e/xHx/wj/AxBiFhgRGxdCEBMhBxKCGR3zGhghFQ4TEg04GyUWL//vFBATDhhBEBUhDxZRHRohGxchHh3/JBr/FhL/DBz/HSQfLxvhGBMTFhkvJCX3LxHkFxMUGBohEg81Df9vIx4xHRk/GhkfHB4xIiAhJBvxGRzx////Ih8hIB0hHR4RDf+vIyIiISAhGh0hHh8hJyExLyTvJyo1JiQfGyBBHh8yKCc0LiGRHR8iDSOh/yj0JyJRHxIm////FBr/HSD/Ji7/LyX/Ki4lL//fFBs3HSRPJy4WLyTvGiFBHyIyJiMV/yjxLDIlKi4lIiM0/ynxKy0SMixRIw0+/////zP2KygRMzIjMC5EJiI2Jywh/zP1LSwhKCMVKf8fLTIUNSpxJyMm/yjx/zL0NSphLCgSK/8vJSZWKjBBNf8/MS+Y/xv+JS7YMf8v////Nf8v/y7xJCb2KjJBLxsuJS7p////////Ki00KzNhNjQhNTAxLC0z////////NjIhMDIRLTNBNv8fNzUh/zfxODE4MComMjQx/////zfyNC0VM/8v////ODEnNTIUNP8vMDVDN/8v/////zH1czyJxUAFMQpujMUADxMLZ43JwAgWDG8I6qAHFAZzBepgDRMLbgbqgBkTC3IE+UAQNQ13EA0hDhcKdgkZQRMuC4CJScEVJgVwD0pBDxcCfAJhoRgZB3AQbgEOFgJ1kHaBEhEGfpF6gQs2CHOMmcEEPgtviZ3BFwoLcY2loRESCISNrsENGAl+BcJBCDsRaQXJwQ4iCIQW2gEKLRF2iuYBDhcEhQvpQRAZEoMI7iEMFgmDFRlCDSUKiBcaQg8aC4aTVqIOGQqHmFaiExoLephaQhEWCIKQasIOCQyFCHKiDQoKhJJ9ohMiDniIhqIQFAh6Da0CEh4ScA+xQhU9DHMCtUIYFwp1FbliDRUKcxjKwhE0FmqRVeMVFwtuhWIDGSsLbI9moxsbCW0MiYMbGAduE42jFRoOagqNIxgfEmqYtcMPSAZtE7XDGTsOaJXJQwQ/CX4W6aMSNgZukRUEBTkLdZkhBBc4FXOWKeQZIQ9wmS1EFA0KdolCBBcVDXoCRcQUDA17DGFEFhMQgAVlpBkgC3QUioQWLRV+mKlkFDIIeJf2pAwpFnPQAv////8C8QMPFf////////8F8QYKFAQCEf////8E8QcOFAMAEQ4TJg//XwD/HwIEEgYHEQ4DQgL/H/8B8f8k/AsIMv///////wgNEwoHMQQBEf8F8QoMEg4DMQQBEv8G8QkcGQ0KMwb/H/8F8gj/HwX/PwsjGBENMg0UFAwOIwcBFAYIM/8k+RAN8gn/HwX/PxESEhgOUgIHMgoNIgYIMwUJYiQclxEKIQMEJAoMMhIYFBUPQ/8A9QMOUxMvHv///wn//wv///8k/xwR/woGJQ0QLyQdZhcUIQ4MEgoRQRQWEhgVMxUlFS//7w8DFgcOYxcaEhYYEhIMEgoRQRkvHv8T8QMOdBIYMQ4SMhQXERobJBkYIRwdExoWIRQMExEQLxkfFC//7xUOFBIWMRsfEy8T4RgWEhQaMR0bEy8Z4RYUIhccIRkaExEdgiEeER//LxcNFxAk8iMgMSEdMhoRFhAc8iIhIh8eMhkbIREdgiEtGCUfQSElEi//7xUZMxseIR0cERAk8SMnFiIhER4aEx0gISImEi8l4ycrJCYlEiEdEiAjESgnMy0igSAQH/8k8f8o9CcjQSAQHwX/zy07Ti//zxUfQiEmMictFi8l4iEiISAkMyYjEyQoQSwrETAxTSckFP8p8SouEiwrESQQP/////8q8S4oIf849i4sESgpEf///zMyEjAtMyYnMSgsES4zEjIrMSckFSgqESUmRicwQTQ7+jEvh/8z8jIrMSwoEir/H/8V/iUtxzH/H////zT//zsxqC0mFisyMf8v8SUt2Dv/L////yssIy4zMTg1ETY0/ywuIv////848TcyETAr/ywy/zY6/zsx/zQy8S4zUTj/Hzc2Hzc5/zo7/y00/ys1//858To7KTYr9TU4Ef////858jUuFDP/H////zoxJzY38Tj/LzA2Pzn/L////zsxZDEtKjr/b////////w==</t>
   </si>
   <si>
-    <t>20153</t>
-  </si>
-  <si>
     <t>LIDIA FITRIA NINGSIH</t>
   </si>
   <si>
@@ -169,9 +139,6 @@
     <t>TlQAEKYRAAAKAU5GVBCcEQAACgFORlIlkhEZAAFoAfwB/AEAAP+dAQEfAAAAB/8oBwwZQBImB4UQOoAYSQyZEGkAElAJhpDhQBNUDICmDgEbSwh9HR0hEU4NhyBS4RRaBoQXZiEPVA2NoX2hGVAEgBmCIRwnAn2VjgESVgaOEsWBC0kOjJ/qwRVTBYSVCYIPVwaUGREiC1ESjaEqAhc/BHUeRoIJPhuIJW2CGUUOcimBQhNZBooAhkIGLxR9iIViCjcXhyCJwho+EHcqlcINVQuNJ7LiCC8ehSe1QhBbCJFg9qIHJGqDqfkCFVIDjToSwwtRDZcqQSMQVgeeMVajDlAIoEt1YwxME5ZVyeMNUh2cqtJDFE4ChSzeow9BD6JFKsQOHm6N5FKkCUEOi/NWxAxCF4OSVuQPICqGrVVEEToYi/mRBAlHCYoG4AEEAhMH/6//////AfH/BPIDAHH///////8EAxML/8//APP/AfT/AvMBBHQGCiUF/z8B/y////8JCBMGA1QKDSgH/z//AvYDBjEMDSgKBTEDASgECFIMDRQL/0//AvgFCjEBBGP/CfIVD1UMBlL/EfYMCGIE/x//////BfIGCDYMEhUNB1ENDhMQ/0////8HCkUGBCgI/18PEhUNClH/B/QKDFUSFhUQDlMWFCQQ/y//C/MHDXMMCBX/EfH/GvUSCkEUFxMT/x//C/QOFiH/GvYSD1EICVb/FfEaHBcYDUEKD1QR/18XGRP///////8LEFH/EPEOFkMYG1IXEyH/IPoaEXEMCRb///8cGxQUDjILDVUSGFIeGSL/E/H/FPIWG0EcHTQbFmINDEgSGkP///8TFzIWG3Mf/28SERYV/38gIUkcGGMk/z8ZFzEWGEYcHkEhHzUdGyQYEjcaIGEfHiMZG2IYHEL/IPMj/x8ZG0EYHXMhHzIj/x8eHSIaIbIiJBEaFUr/////JvUhHEElIhH/H/IdGhkg/0//JPH/H/EhIBYl/x8k/x//J/L///8ZH2El/x//J/EjGRcfIhEiIREgJmH/////JPEhIBX///////8lIhH///////////8jJCEBBFz9ogcBBwAspA7///8ABAAA/ykNHcASJQeJDkLgGEgMl45iwBsTIHoIaiAMEweCE22AEk8KiI3VwBJUC4OmBqEaSwl/HymhEU4OhyFeQRVcBYegbSEZUAWDGXKBD1ILkJKCwRFXBo4UyQEMSQ+Rod5hFVYFiJT9IQ9ZCJccGaILVA+PnR6CFjsFeSFO4gk+G4l8eeIJNhqJA37CBjIVgSx94hlDD3UqjaITWgaMKpVCGzwPeCuhIg5YC48rukIJOSCFKMGiEFsHlKftwhRRA45aAkMHJEuCXBXjBxtHhDoiAwxPDZgrTYMQVwefMGLjDlAIolKFgwxIFZeqwgMUTwGJXNUDDlIhnDDq4w9DDqHiRgQKQg+KfUpEDx9Dh69JJBE7GIz9TkQNQR2E+o2ECUkLi+wBBgQSDAPT/////wHxAgYTBQBx////////Af8f/////wbzCACRBQoXE//v/////wTxCAVSDAOx/wDy/wH0AwQSAQZ0CAslB/8vAQIz////FAlzCAVkCw4nCv8/AwVCBghhDRU4CwdBBQEpBgliAQZj////FBBFDQhSEA4UDP9PAwV2BwsxAwdiBgiUDRUVDgpRDg8SE/9f/wP6Cg1FCAY5CRZSEBUVDgtRDAoUCw1VFRcUEQ9SFxITEf8v/wzyDhUiDQkV/xbyFBUUGQ50EhgUE/8v/wz0DxchE/8fEQ4WFx0iGP8vGBsk////////DBJR/xr1FRBBCf9P/xbxGh4WGQ4xCxBUFP9P/yH6GhRhCf9P////Hh0UGBJCDg1JFRlBIBsj/xPyERJCFx1BHh8kHRdhDhA3FRoyFRAVFP9fISNJHhlS/////xP0GB01HP//////Gxj/Fx3/Iv//IP8fHBjxFxlGHyIxIyI0Hx0kGRolFiHBIiAjHB3zGRpIHiEk////HB3xHyE3IicTGhRJ/////yb1Ix5RJP8fIB8SGiOiJSchJSciIiAjHxoZIf9fJSci/yjy////HCDxJyISIyEnJv8f/yjxIyEV////////JSIRJf8f/yjxJCAjIiEY/////////xv4JCch/yAPOuAYRgyrGE0gFSUKrRZpYBJNDaeO4WATUQyiogoBG0sIlx4lQRFODqkhUgEVWgWmEnKhD1QOsY1+YRFWCK6gfYEZUASiGcKBDEARs5/moRVXBKSVBUIPVgi0HR3CC1AUsKAuQhcwA5aeOUIWJwWZKXbiGD0KlSR6IhsxDpYskaITWQaqK6lCDlkNtDG9YgpAJKoovYIQWwi1qumiFFIDsT4e4wtREbopYcMQUwi/LX4jD04NwlSFYwxJGLepzkMUSgGtW9GjDUwmuNs95Ak6E6jzWuQMQB+m+pFkCUgMrIAB/wTyAwFy////////BAMVAv8v/////wDyBgND////////AQAk/wLzAQRUCQYSBf8/AP8v////EQljBgNUCwgSCv9v/wL2AwYxCxIoCAUxAwEmBAlSCwwUCv8//wL4BQgx/wXyAwZTCxIVDAdRAARj////EQ5FCwZSDA0T/////wL7Bws0BgQoCRFRDxL1DAhRCgcUBguFEhMVFA2DExQl/////wrzDBIzCwkV/xHxEBYVDwjxCwn/DhD//xb/Egz//xb1Eg5BCf9fEf8f/xv6EA4RCf9P////FhgXFQxBCA9fEP9PGBcUFA1CDAtZEhVSGv8v////DQxYExdBGBk0FxNiDA9PEhZDEhAVEf9/GxhGFxWTHf8v/xTxExVGGBpB/xz1GRckFRY2/xvx/xzyGhcyFRhC/xvz/////xfxFRlzHB0hFhBI////////HBhhHf8fGhkiGBtW/x7xHB4S/x/z/////xrx/////x/xHf8vHBsW////////////HR4xsicQRmAZRQ6mGlVgFSUKrpBmoBsVJIsYdQATSg2njNWgElIMpaH6gBpNCpggLcERTQ6oIWJhFVcFqIxyARFUCq6gcSEZTQSjG34hEEsMsRvKAQ08ELWf2kEVUAWnmfXBDlIKth0hAgxQErAqhmIZOQuXI4qiGzINmCuZAhRVBqsqtYIOVwy1KMnCEFgHtjDN4go8Ha6m3UIUUQOxZ/FCBxJMomHxwgccZ6Vo/oIHElOjUgGjCBlhqGEdAwgkRKM7LgMMURG7KmXjEFEIvy6OYw9BDsJZlYMMPxq3qrrDE1AAsmLdAw5DKbct/iMQORi31zlECjsUqK06BBEtHK18SiQPIE2n/E5EDT8upvyN5AlKDqzUAQIFEwQBcv///////wUEFAP/H/////8A8gD/H/////8F8wcBkgcEQv///////wECFP8D8gEFRAcMJAb/LwACM////xAJcwcEZAwIEv////8E8gUHYQ8MMwgGQQQAKQUJYv8D+AYHJAwRFQ0KUQEFM////w8RWQwHUhENRAv/T/8G8wgMERIOU/////8E+QoNQQYHEwkQUg8RFQ0IUQsKFAcMhRMSNA7/LxIUFP////8L8w0RIv8c+hEMQQn/XxD/L/8f+xEPYgn/T////xUcFhMNMQwJWQ//TxwbFBT/Pw4MGRETQRwdJBsSYQ0MOBH/PxsZHxf//w4NRxIdMhEJGQ//Xx8cRRsTkv////8O/xcZ/xj//xb///8O/xQZ/xoY/////xYX/xkb9Rr//xoY/xcL/xQb/x4i/////xgZ/xQb/yL//yL/LxkU8RITRhweQSEdMh4bRBMVJf8f8SEgEh4bMxMcQh//T////xob8RwdQyAiERUPSf////8j9SEcUSIaHx4dEh8hYiQlESMkEiIgMh0fFf///yAlEv8m8v///xoe8SEfFf///////yQgIiUgESEjIv////8m8ST/H/8m8SIeIyAhEv////////8a/yIlIfMpDDpgGEoNghBpQBJOCW6Q4WATUAxnqRYhG0YHaxshQRFMDm8fUuEUWwZrFWpBD1QMdRt+IRwjBWihgcEZTQVnlIrhEVYGdRPJwQtIDHSg6sEVTQZtlgmCD1MGeBgVYgtRDnYgHoIVHQJrmioCFzoDYBpKogk8GHGpTuIVIAJmJ2ViGUAQXoqBQgo4E3L8hkIGKhVpKYliE1gGcx+Jwho6E2MrnQIOVQp0J7lCEFgHdy+5ogpDGXCp8cIUUARzQfrCBxtubjoa4wtSC3wqPSMQVAaCMVKjDkYGhkZ5YwxCEHswymMPRAyIUcnjDUYXgavSQxRMBW9IGuQOHjd7lU7EDx4uceVS5Ak+DHatUSQROhZz71bEDEIUbPiRRAlFCnXsAf8D8gIBdP///////wMCEwr/z/////8A9P8B8wADdAgFEgT/PwD/L////wcIEwUBUQkMKAb/P/8B9gIFMQsVKAkEMQIAKAMIUgsMFAr/T/8B+AQJMf8S9gsIYgP/H////wADYwf/LxYPVQsFUv8E8gUINgsVFQwGUQwNExD/T////wYJRQUDKAj/Xw8OEQwJUf8G9AkOVBUXFRANUxcTJBD/L/8K8wYMcxEVFBgMdAkLEQcPcQsIFQf/bxIaFREOERMbFRT/H/8K9A0XIQ4PERIWIyIVcxgMY/8a9hUPUQgHVv8W8f8Q8Q0VRxcZMhsUQRMbE////////wEQ4RodFxgMQQkRUxL/X/8i+hoScQsHFv///x0cFBkNQgoMVRUYUh0eNBwXYgwORxUaQxwbE/8U8hMMKBceQhURFBb/fyIgSR0YY/////8U8xMZQxwhNif/PxsZMRcYRh4fISAhNR4cJBgVNxoiYSAfExscYhgdQv8i8yX/HxscQRceUyAhMiMnEiEfIx4aGSL/TyX/Hx8eIh0gUiMnERoWSv////8m9SAdQSclERshcSAiFiYkESMgESImYf///ygnESf/H/8o8v///xshUSAiFf///////yQjEST/H/8o8SUbFyEjEf///////////yUnIfwoDELAGEgMgRJxwBJNCnCP2eASUwtrqQrBGkcIbR4poRFLDm8hXkEVWgduGXbBD1IJd6F1QRlOBmqTfoERVwV3HYqBHCMDahXJQQxIDHih3mEVVAVwlf0hD1YHfBsd4gtUCnmdHoIWNwRlJiriFRwDaKNCghUhAmkfTgIKOxdyLnHCGT8SYYN5wgk3FnMDesIGLxRrK43CE1gHdCmZQhs4D2QrqUIOVgp3KMWiEFgHejDJ4go/FnKp3WIUTQN4SgYjCCFYcFoVAwchNnA6JgMMUwx8K0ljEFQGhDFeww5QBolMiYMMSRJ7qcIDFE0EdDDSow9EC4hZ2eMNThx/r0HEEDkUduVKRAo/DXWYiYQSFAx2+o3ECUUKduAB/wPzAgF0////////AwISCv+//////wD0/wHyAAN0BQglBP8vAP8/////CQcjBQFhCwgSCv9v/wLyAwVhCxU4CARBAgApAwdiDwwUCv9P/wL2BAgxAANj/wnyEg5FCwVS/wTyAwWUCxUVDAZR/xL2CwdyA/8v////DA0SFP9f////BgtFBQM5BxZSDhUVDAhRCgYUCAtVFRcUDf8vFxMTEf8v/wryDBUiCwcVCRJx/xX1DwwU/xDxFwiCCwcmDhIRCw8hCRKC/xXzGAxjGRMxFP8v/wr0DRch/xr1FQ5BBwlG/xbx////EQwWFxkhGxRBGRsU////////ChNRGh4WGAwxCBBTEv9P/yH6GhJhCf9v////Hh0UGRMyDQsZFRhBHh8kHRdhDBA2FRoyHRsT/xPxEQxHFx8yFRAUEv9fIR5FGBck/xz//xT0GRc3HSVG/////xT/Gx3/I///Jf8/GxlBFxhGHyAxIiM0Hx0kGBolFiGxIiATGx1zGBpIHiEkJf8fGx1BHx40IiMxGhZK/////yT1Ih5RJCUTIyAjHxoZISZfJf8fIB8SGiKiJP8fIiEV/yb/////JSNBIiY//yfy////HCPxJCH//////////yX/Jv///////xz/JSMh</t>
   </si>
   <si>
-    <t>6735</t>
-  </si>
-  <si>
     <t>ANNISA KHUSNUL S.</t>
   </si>
   <si>
@@ -184,9 +151,6 @@
     <t>TlQAEB0PAAAKAU5GVBATDwAACgFORlIlCQ8ZAAFoAfwB/AEAAP+1AQEfAAAAB9kgBwhWYBAkC4+VyiAXSAeeHe3gFUYHqAMmwQ1VEbKMVmESVg+2fG2hBR8EjyqCwRs4CJn2qQEMRg+nIeLhD0ggrSMVIg88JqasFSIaUwGWVi1iBk0GphVW4gw3NJtQeqIGOgavMnqiDThumluZYg0pVZzVugIHSQStTt7CDSwUq1DxwgwoDqvUHgMLMAeltC7DGEsEis5Wows7CqJFnqMUUAeKLaKjBjsPkzeqgwVODZlVsoMPTwebO8XjA0UJlpkRhAohUYDZLgQLKSGBaHLEDToRe/KB5Ag1L4AM4oQHExN/BoABAgQ4A/9/////////////////BgoVAgAhCgg8BP9vAP8/AQYhBAgXBwVP////AAJ1AwAYAgZnChQzCAdj/////wP/Bwv/F///FAp0BAFx////////CAk1DAtiBf//AwRDFAlCCwdDAwR2BgrZGQxSCwdlAwiSChTGAgY0////FBZJCAST/////wX/BwwnEw2SDg8fEA01BQf2CQou/////wvyBwwVExBxDxPxEAxBBwmEChbnEA3/DA7/ChT/ERL/DBI3ExdR/////w3xEhAWDQ+PBBTsFhmEExAXDQ+fERQeGRVhEhYbFRsUF/9PEA5RCv9P/////xb0EQnGEhYZGRtT/xf1EBNhHRlFEQ6HFP9P////Hv8vGP8fEBMUFRtRHxoi////EBUWFxsSGxc4FRFUFBaF/x3x////////EBgiGx5UFxUTGf8/HB4T/xjyGf8fHR81HholGxUTHhwTFRlx////////Hf8f/x/z/xjyFxwi/////////xryHv8/AgRVlWIN1wVkCgAHAAQAAKYkk77gFkkInR/1QBZFB6gJHiEOVBG0hkrhEVUQuWJ5QQUpBJAkiuEbNQia+51BDEsPqSPqQRBEHq+sCeIZUwKaJxWCD0ciqFU1AgZRBqcbVkINPT6bT4JiBkAGrziGAg47WJ1TjQINJ1Wa1q5CB0sErk+ygg0dMKFQ6oINKhKsS/1iDCsIrNYOQws6Bai1HqMYSwSOzUbjCzQHp8qBQwohJJDDicMJHSeN1qqjCh4mikauoxRQCIsqsuMGOw+UuLWDCRwziDa6owVODJxXwkMPUAiZPNEDBEUKmaQZ5AkfYH/ZImQLKxeCboJkDToReuuFZAk2NIEF8uQHEhCGsAH///////8FASIDAocIBywD/2//APL/BfEDBxgGBE//////AfUC/x8AAYYIFDMHBnP///////8CBv8KHv//CPQHAeEA/y////8HCTQOCvEE//8CA0MUCVIKBlMCA4cFCOkBBST///8UGUkHA5MdC1IKBlQCB5IIFLf/////BP8GCxcPDDINDi8PCkcGA2oJFCr/////CvIGDi8PFy8QDi8PC2IJCE4UGcgaD/8EC/8JDf8QEf8LElcTGmP///8MBC8SDxcKDq8JFG4ZEaESDxgMEKEIFO4ZHaUWE/EPDn8QEREZFbESGR0VFi8a/18PDm8I/0//////GfURCecRFB4dH2MW//8PE3IVGf8dGP8bF///D/8VFv8dGP8bGv//D/8UHeUhH3IbGvQWFfEhHVYRDagU/1////8i/y8c/y8PFTYbH/EXGP8dIP8f//8aD/8jHjL///8PFy8aHyIgGCUVEGUUGab/IfL///////8PHCIfIkIbGPIdIDH/IvL/GvEd/y8hIkL/H/EYFTQiIBQdGSX/////I/Ih/x//I/P/HPIfICL/////////HvIiITKjGxBWYBEkDaCSvqAWRwm3IOqgFjoHvgwmgQ5SFd2HToERTxbWApLhDD8VzimiQRwxCLIp/cEQLSHCqQkCGlECuSctQhAwIryYMmITIQvAJ0ECDiZDuVNFogVIB7XapkIHRQjATa5CBSwHvT7OwhMhCr+0IqMYSgWwWUUjDBsHvkluYxImCrXFjcMJKSOwR7KjFFAJri/KgwVEELUZygMHIRKwXtYjD0gKtTfegwQ2DbbrbiQJLUGhboEkDjMVmkQBAQQYA/9/////////AP8f////BgIRBP9/BgccBABi/wHx////BAcYBf8/////AAJ1AwAYAQJ2CAc3CQXyBwtGDQwv////AwQy/wj0CgLB////////Dwk/DQU0BAJ8CAqxAgY0////EA9JCgSDDxH/C///BQf/ChD/BAJLBgjIEA8xEQfxEhE/Df9PBQdjCQ/z////////BQv/DQ7/Cw9NERbx/w7yDAXy/////wz/BQ0iExViEhEfCwoxAgjJEBRBCP9P/////xT0EQ/0Ew7/DQv/DxL/Fxn/FxEvDQrSDxAWFP8vERL5Fxl1/xbz/w30GhdFEg8hEP9P/////xjx////DhEvFhkRGf8fGBUxDg0xExc2GRMnEQ/zEv8v/xry////////DhURFxmSGv8v/////xXxFhcRGRMoFxQk////////ciUTVuARIwygkLJAFkQKtiH2wBY3B78SHuEORRXefT4BETsV2giOQQ0rFtGo+YEZTQK8KwniEDkfwJUqAhMhDcBTRaIFRQe1K02CDiFFuKBi4hEVEbtVhiINHlm1P4aCDSRmtEOWIg0QTLXbmoIHRQjAQZqCDhQ/tku+wgQjB73D1gINEhq4QeIiFCIJv+DtIgwbDbu0DoMYSQW1UREjDC8HvlgWIw0jCr/aduMKGxm1yHnDCSkcs0t+YxImCrXQjkMLJBqyu8GjCSA3p0nKoxRQCK8S1kMHIBKuxNVjChBFpC3e4wVCErRf4sMORwqyNO5jBDUNteZypAkqQ6BwiaQNMhaYvAEBAxgJ//////////8A/x//////AvIE/48GCDwE/38B/y////8EBxgF/0////8AAoYD/x8AApcGCDYHBXMHCkYJ//////8DBEMC/z////8VE0kIBIQLChIPBTQEAn0GCJEFBDb/BvgVE0ILBzH///////8FDP8PEf8QDSIP/z8FB2ILEyMHCBMGFaYTFycQClIeD1X/BfgKDSEaDnEODxYM/x8KCyUQGhYSDxYJDPENCxYQFyEKFD8WHvMR/z8JBfMSDygNChIHC1UTGmX/////Cf8FDzMZIGMOCxcTF4EU//8PBWkaFygQC2IG/58VHVESGv8XFv8iD///Dv8G/0//////HfUTC1YZEf8PFP8QF/8aGP8YFi8UEvETGochG1EXGhgbHB8eGVEPFm8WGPEbHB8eIjURD2QhGzcXEHUTFScd/z8XGhchH18cIvcZGBEZG/8hH/8jHv//D/8kIUYaEzEV/1////8j/y//IPL/EfQZHD8bIf//JP8jHv8cGf////8i/y8RGTQeIyIjGyUXE1Qa/z//JPL///////8RICIeI0QdJGL/////IPIeHy8jHy8hHST////////BIJbKQBdICIMc5aAVQQeI/iZhDUoPi5Be4RJIC5NwacEFMwN8KYlhGzcJgfKpwQtFDIga3mEPOBmGHgICDzIgg6wVIhpQAXxYKYIGUAWIDVbCDDclfFBywgY8BZUyfuINNUd8X5liDShXgD6dgg0iTYHRxuIGSQKPUsrCCyEKjE7OAg0vHI/SJsMJLgqItSrDGEcFc9BCowohD4nPXoMLOAuGOaaDBT0KgC+qwwZMDXxGsqMUTQhxVbajD1EGgT3J4wNECIDaKkQLKB5yoULECR1KZ2BqxA05Dmz2hQQJMS5ngAH///////8FFCkB/y8FAxYC/1////8A/y8DBxcGBEP/////AfX///8BBWcJFDEHAmH///////8GC3wK/28UCXQDAHL///////8HCDQLCmIE/38CAUoUCEELBjMC/38DCWkUDWQLBiQCB4EFCesBBTT///8UGUkHA5P/////BPYGCycRDJINDh8QDDUEBsYICS7/////CvIGCxUREHEPDh8MC2EIA00JGegRDP8LDf8JFP8PEv8SERIMDp8NCR4UGtQLETUTF0H/////DPETEBUMC3IOEvEaFYETESEMDo8NFB4ZFqERGR4VHBQY/z8QC0EJ/0//////GfQPCNYSGRwWHBQY/z8TEREDGeoaHFMYF0UVERL/G/L///8QExQYHREf/y8X/x8QFRMaHXEeGkUWDagU/0////8cGBcWD1QUGZX/HvH///////8QFyIdH0Qa/x8e/z8dFxMYFiMYFhQcHhP/H/L/G/QfHBMWGnEZ/0////8e/x//////GPIdHCLDI5TCIBdJCIId7eAVRAiJBB7hDVIOjo9aoRJMDJRhcaEFLAR9LZHBGzcJgvehQQxHDYsd5sEPPRuJrQnCGVABgCIKYg87HYZXMUIGTwaLE1YiDTQtfFF6ggY7BZY3ikIOMzWAQanCDSMzhNO6IgdLA5FQ0oILIgmPTfGCDDoNmdMaAwouCY21GqMYRwZ30TbDCiwLjs9WowsxCorJcgMKIB952JrDCiYddTiygwVFCoQttsMGQwx/VMJDD1EHgUbCoxROCHM81QMEQwmD1eLDCg45bqvqIwoTQmvYHqQLKRF0pjpkCR1IZmZ6hA02D2ztiYQJMS5npAH///////8FCCUBAicFBxwD/2////8A/y8DBxgGBEP/////AfUC/x8BBWcIEzMHBnP///////8CBjYKHFgTCHMDAXH///////8HCTQLCmEE/28CA0MTCWIKBlMCA4cFCNoBBSP///8TG0kHA5MaC2MKBmQCB5IIE7f/////BPUGCxcQDJINDiMPDEYEBsYJCD7/////CvIGCyYQD4IOEBMPC2IJCF4TG8gREPIMC5MNCB4TGtQLEEYSGVP/////DPISDxYMBogOEy4RFPEUEv8QC/8OE/8bFf8QEx4UFiEZ/08PBlcI/0//////G/UNCccRE/4VFiEZ/18SECEOEy4aHWIW/y8UES8UFRIXHSIZGEX/EvETGuUhHXEZGEYWFSH/HPL///8PFiUZICIi/y8Y/y8PFiQXHkIfFyUVDmQTG6b/IfIhGlYVDbgT/1////////////8PGCIeImITGtQfICIeGRMPF2EWFzEdHxIiIDIcGWIa/y8hIkIgGCUdFyMZHhIfISQi/y//GPIiIBQfGkL///////8h/x//////GPIgHyI=</t>
   </si>
   <si>
-    <t>16027</t>
-  </si>
-  <si>
     <t>MUHAMMAD AKBAR DWI PUTRA</t>
   </si>
   <si>
@@ -196,9 +160,6 @@
     <t>TlQAEGANAAAKAU5GVBBWDQAACgFORlIlTA0ZAAFoAfwB/AEAAP+iAQEfAAAAB/8dB+pu4ApGBpN6/QATTBKbmwmBGkkJkecdoQlPBpgnUoEXQAqbHGJBFFIQmeyRgQxZB6adpWEYRQiiZsLhDjgTnfX54Q1CEpmjDQIYUQmY5hZiCzwFlXVW4hBIIIKLhgITPhp73dKCBkQIhaMd4xpMCIfjIQMIRgiJ50qDCTwKifpWwwtPEIiRVWMRSw54nXnDGFAJgpqRAxVSB3/0qcMHTAaHgfFjDkkIcPwKhAg/CX+OFUQURQx2jVnEGDwLdn555Ao+A3SE2eQWJgZ1BlwB/wH3A/9P////////AP9/////BAUTCAZj/////////wf2BAFEAQY2Cw6I/////wD0BwwaBQEh/wL0////CgwXCAM2Af8/BAchBQgjCQ5T/wP2AAGjBAIW////DwpTDAWRCwYTAAHWBQozDAlBCgwzEguB/wb1AAjhBAdD////DxM7DQhjCQwTEg6B////AwaDCwkzBQp2/w3xExJkDAUXCv9vDxM1EhAyCRIXEP8//////wvxCv8//////xT0FQ1zDBEiFv9P////Dgs0ExIRGxaS/xDyAwvmExcUGBZBEQ4XDA1DCw2VChS0Ff8fFxJRDQ8U/////xr2FRM0DQpKFP8/GhlEFxNRFxs3GP8/////EBFCFhI0ExVVGf8fGxhBGRsT/////xbzERdREhU0FP9vGhwV/xfxGRQW////////HBdB/xjzFxlEHP8v////FxlVGv9P////////AAQABwAEAAD/H+xmIAtGBpR3+YASUBGemgEhGkoIkugV4QlPBZooWsEXQAqcH2qhFFIPmu+F4QxZB6ibmQEYQgiiZcKhDjgSnvvtQQ5GFJqhAcIXUQmZ5QrCCz0Gl25SYhBOHYV/eqISSR583sbiBkYHiRv1QhAeN30ZDWMPQDWBpxFjGk0IieEZgwhKCIvoPuMJPAqLhEXjEEkRegBOQwxOE4mfbWMYUgmEnIGDFFEJf/WhQwhMB4mA8cMNSQdy/AoECUAJgI0NpBNFDHWLTQQYPAl3fHVkCj4Dd4XZRBYpBXd0Af8B9wP/T////////wMAJ////wQFEwkGYv////////8H9QQBQwEGJQsOiP////8A9AcNGwUBMf8C9P///woMGAgDRwH/PwQHMQUIIwkOQ/8D9QABogEEEf///xEKQg0FkQsGEwAB5gUKQwwJUQoMMxAL8f8G9AgFFAQHQv///xEPLw0IYwkMFA8O8f///wMGgw4JMwgFWAoNYQ8V9QwJEwUKhhEXNA8V9AkVGBL/P/////8L8RQZ/xAO/wkN/woW/xQZ/xUS/wsM/w8W/wr/L/////8W8xcNYxAT8hoYc////w4LNBAV8hoYYv8S8gML5xAP/w0RVxcbExkVQRcZFBoYURMLKQwQXw0RE/////8c9RcUIw8K+Rb/LxwbMxkUQRkdJhr/P////xMVIRgVJBQXRBv/Hx0aMRsdE/////8Y8xMZYRAX8xb/XxweFP8Z8RsWFf///////x4dMv8a8xUZgx7/H////xkbRBz/P/////////8Z7mZgC0YHtnP5IBJOFcaYBSEaSAq26hUhCkwGuiRyQRVNELnzgUENVQ2/9t3hDEUQuJ79wRdJCblxXgIRSiiniYriEkAiod7WggY+CasSCUMPPTWi4hHDCEYKqqYRgxpLCa3mLUMKRA2nEC7DDhMsoo5VYxFPEZn4WgMMTBSnoH3jGE4Jp5mVIxVTCKH2qQMISwin/gqECD0JnoMSpA5CCI6MKkQUPAuVfGZkCzgDkSwBAgFHA/9P////////AwA3////AgRDCAWj/////////wf4BAFkAQU2Bgr4////AP9PBwgXBQMmAf8/Av9vBAgnBgrz/wP2AAGjBwj/Cwr//wP/BQH/BAIY////DRA7CQZvCgYvAQem/wnxCw5CCAEaB/9vDRM0Cw4xCAwjFP9v/////wb/EA8hEQ4S/wj0CRIyCw5CFhR0/wrz/wb/B/8//////xL0EwlzDxEiFhRj/wzyAwjiEBYVEQ4S/wj0CxITDwkVBxK0ExcUFhFREBYUFRRB/w7yCA9BCQ0U/////xf2ExA0CwcaDRJz/xf0FhBRFhg2Ff8/////DA5DFhgS/////xTzEQ9FFBE0EBNVF/8f/xjyDxNEEv9v/////xbx/xXyERZy////////1xzvWsALRge3l/WgGUkKt3EBgRFNFMjsCWEKSQa793mhDVUNwSV+YRVKD7grfUEYLwy6lY3BFz8Muvbd4QxDELic9WEXSQq4alJiEEwkqnd6ghItJaLgxuIGPwetGP3CDzw6oeMBQwlHCauoCSMaSAmv5yGDCkQNpxkmQw8SMKCQRcMQTRmbA0qDDE0Ypp9tgxhNCaiYhcMUVQqh+J2jCEsJqAAGJAk+CZ+ABgQOQQmRjCKkEz8LlI5ZhBg+Cpd/bgQLOAOSUAEBAkcD/0//////////////////Bv8FAmMDACf///8BBTMKBKICBCUI//////8A/08FCicIDPP/A/UAAqIJChgEAiP/AfYGB/8JB/8FAv//Af////8CAf8G////Cf8LBf8JCv8ODP//A/8EAv8FBx////8PFCYLBGIMCD8EBXgJC2ENEEIKCB8FCYYPFTQRDVMKDjMW/2//////CP8SERETDhMICvQLFDENEDEXFnP/DPP/CP8J/y////8aFPMSC3MREyIYFmL/DvEDCtIZGFYTEBIIDfEJEqERDREJFKMVGRQYE1EVGBUXFlEQCC8KEVELDxP/////GfYVEiMNCSkPFGIaGfQYElEYGzYX/z//DPYQEyEYGxP/////FvMTElUXExUSFVUZ/x8b/z8RFVQU/28a////GPEZFP//////////GP//F/MYGTP////////gIOluwApCBnl9/QATSQ6BnAVBGkcIdeYdoQlGBn0IOcESGw2FhUKhFBoOgyVSgRc9CYAaXgEUTw2D6pVBDFYGiaCpYRhCCIZkrcEONg2H8grCDT8PgaMNIhhPCXzkEoILOwR8dVLCEEkdao+KIhM8FGjd0qIGQwltEfnCDzg0ZwARww4QKG6kGaMaSgdu4iEjCEcIc+c5owlBCXb3VgMMSxBzklVjEUkNY5x5wxhOCmiZkQMVUQhn8anjB0oHcIX5ww5ECVuOGYQUPwxg+CFECCsJZ45dBBk2DmCAeUQLNQRegAH/AfcIA7T///////8A/3////8GBRIECPP/////////CfYGAUQECvkIEGj/////APQHD/8KCP8AAf//Bf8AAZL/AvUGDBMHBB8JDhoHBSH/AvT///8MDhcKAzYEBfECBmIECvMLEFP/A/YAAbMGAhb///8TDFMOBZH/CPMABO8HDDMOC1IMDkIREHENCBUKBC8GCUP///8TFzsPCmQLDhMREIH///8DCIMNCzIHCXkMD2ERFkQOBxcM/28TFzURFDILFhcU/z//////DfEXGycSFfINDoQPEzYXHP8bFv8QC/8OEf8M/z//////GPQZD3MSFfIdGoT///8QDTQSFvIfGqP/FPIDDeYXGyQdGlEVECcOEk8RDyUMGLQZ/x8bFlIPExT/////HvYZFzQRDBoTGHMeHEQbF1EbHzcd/0////8UFUMaFjQXGVUc/x8fHUEXGUQY/28e/x//G/EbHxP///////8aEk8cGBb/////////G/EdGjcbHET/////////H+pmQAtFBnx3+WASTQ2Dm/ngGUcHd+cV4QlMBoAoWuEXPwmCG2phFFENhO2JoQxZBoufnSEYRAiIYblhDjcNiaP9wRdPCn32AgIOQBCC4grCCzsEfm9OQhBNGW2EfsISRhlp3cYCB0QHcBr5QhAnNWYZCUMPMjJspw1DGkwHceIdYwhFCHXnLQMKQwp5i0kDEUoNZf1KowxOFHWdbWMYUAlrm4XDFE8JaPWdYwhKCXKD9UMORAhdjQ3kE0EMYf0ZxAgzC2mMVaQYOQxifXnECjoEYoTZxBYkBmt0Af8B9wP/T////////wMAJ////wQFFAoIdf////////8E9AUBYwEGJQsOiP////8A9AcNGwUBMf8C9P///wkMGAgDNwH/TwIEYwUIIgoOU/8D9QABsgQCFf///xEJQgwFkQsGEgMBhQUJMgwKUgQHQv///xEPKA0IYgkMMxAO8QsGJQgFJQoMJA8Ogf///wMIgQ4KMwgFWAkNYQ8VRQwIFQcJlhEXNA8TMQoVGBL/P/////8L8RQZFhAS8woNcwkWgRQZ/xUS/wsM/w8W/wn/L////xwWgxcNYxAT8Rj/P////w4LNBAV8hkYUv8S8QML1hAP8Q0WUxcaExkVQRQZFBsYURMLKQwQXw0RE/////8c9RcUIw8JGRb/LxwaMxkUQRkdJhv/P////xMVIRgVJBQXRBr/Hx0bMRAX8xb/XxweH/8Z8RodEv////8Y8xMZYRoWFf///////x4Z8f8b8hUZgx7//////xka/xz//////////w==</t>
   </si>
   <si>
-    <t>20703</t>
-  </si>
-  <si>
     <t>ANNASTASYA ZEA PUTRICANTIKA</t>
   </si>
   <si>
@@ -208,9 +169,6 @@
     <t>TlQAEBIMAAAKAU5GVBAIDAAACgFORlIl/gsZAAFoAfwB/AEAAP+oAQEfAAAAB9EbB+h1AQdEBZn9puELUg+QXN5BBEUDn2P+QQpcDZsMCqIOSguYDU6iDVEVmGJSQgxTGpXeaoIETAWicAWDDz0slEgqowZICKosKmMQSxmXQzYDDythlaM5QxRJCZI/WgMNPxabOmIjDzQdnjGNAxA5CqeulsMWMxJ1OdpDGBIFcrQCRBA+Fo+xCYQRLjmFbBWkEy8afkg+JBghC3jpTqQRFy59Il4kDTkLlSiGJAtICZbstkQTQR16qAmFDUMHhQZEAf8B9AkCof////////8E8wMCIwD/T////////////wADFQkHkwcCFQABYv8F8wYJMwwIWAUDIQH/P////wwIJQkGIQMBNQT/LwcCWQMEMgUMEggJUQMNHAn/X/////8C8wkGZQX/XwwKMQsNIf////8H9QYLGA0Xdg8OIgsIEQX/XwwQMxcNQQcF1wgKIRAOUQT/X////xAUEw8KYxf/HwkGdgULYQ4SIhf/Tw0FKQsMFhAPYRIXFgkOwQsMFhAUZP////8R8RUUEw8MYRUUFBIQYf///////w8MFhMWERoXhP8N8g8QFRT/PxYXJRIOERMPJQwQMxX/TxkWMRkWExQRQf///////xX/PxkaJxcJORMUIRr/Pxj/Lw0PFhIZQRr/H////wkSRhf/L////////xoXURYVIRgWFxn/X////////wIENTEDD7YhxBEABwAEAADaHeppYQdGBpr/omEMUhCPW+rhA0YEoWIGAgpeDJ0NCgIPSgubEFIiDkgSm2Fa4gtWGZbfYsIEUQWkZfkCD0gvlKEtAxROCJUvMqMQTRWYSDqDBkoIqkE6ww40X5Y0QkMPH0WYPGrjDEsRnzduAw83FqKtgoMWMwx5NZlDED0GprPa4xEyDo4l7oMYCAZ1tvYDEEIRlLX9IxE3JIppKWQTLzN+QE4EGB8NedpWJBInOHwhaoQNRAuVK5JkC0wKl+S6xBNCHHqs/SQNRQaJXAH/AfQDAmH/////////BPQDAjQA/0////////////8AAxYH/08HAiYAAWMEBSQGC0UJCFgFAzIB/0////8JCCULBkEDBEP///8HAmoDAUYFCRIIC1IDBiYL/2////8CAEQLB2sF/1//CvENDCIF/y////8QEhQKCDIRDyMNCCEF/28JEDT/////B/YGDCkOGoUZDkIHBegICiINDxEPDhMMBhgICiIJEVEZ/y8LBocIDCIPFDMU/x8OBjkNChMQEXH/////E/IXEiURCWEUGhgOD0EKCSUQEmEKEBUTFmIYFTELEdH/F/EWEUcQ/y////8REhMVGBIcGYX/DvMREhETFlEcGYUUDxEZFUESECMTF0QbGDH/G/EWEEIT/x////8WFxQb/z8aGXQVEiP/HPMa/z8OFCUYG0Mc/x////8OGUMY/38X/x////8cGVIYEzIaGBcb/1/////////UF+xagQc9CLMBoqEMURG7EvmhD0ANwlj9wQM7BrRfDqIJXQ++FFKCDkcWwuJe4gRNB71aYmILUhy7YQEjDz1OuZ0lwxNNC64xMoMQRxy4PjbjDjJUuEZKgwZGCcg4eYMNORTErZbDFjUQi7DS4xE4C6hVEaQTJRuXqz0EEhhVls5epBIsYpMWiaQOKhKmKpqEC0kLteayJBNBJpat9eQMQwmiFAH/AfQEA2L///////8CBTUEAyMA/0////8JBWMHBDIB/z////////////8ABCUG/z8GAxUAAWICBSMHDDMJCCUMByEBAlP///8ECBsM/1////8DADT/BvUEATUCBTEIDFEMBmsFAln/CvEPCyIF/y////8ODxQKCDMPDRQLCBEF/18JDjMNDBgGBdYICiEOD1H/////BvUHCxgNFIQT/y8MB4cICyEPEUL/////////EPMPCUEK/x8OEEIRExUMDcQRDC0PCSMO/z//EvEPEBL/EvEVEzQUDWIQ/x//FfIWE3MRDxL/FvT/FPMMD3URFUEW/x////8ND0cT/z////////8WE1ESDiIUExQV/1////////+KG+5OwQc8CLQFniENThC6WQliAzoHtBAJ4g8+DcReGkIJVw6+5FJCBU8HvhZeIg89E8RZcuIKURi8Wf2iDjFVuZsdgxNNDLE7QqMOLki5NELjEEQWtzVGQw8nO7lFWmMGRAnGOIYjDy4Svq2GYxY2DpA1iUMNMRDHq77DEScJrrjSow85Cbi3BqQSKSCbUCGEEyMvlq415BEYS5jJViQTI3CSE5HkDioTpC+ixAtHC7TdvsQTOCSUsuFkDEQKqEQB/wH1BAJy////////AwY2BAUyAP9f////////////AAQlBf8/DwZDBwQxAf8/////BQIlAP9/AQY0Bw1FBAcmDf9v////AgA1CQglDQdCAQNj/////wX2BAFGAwYyCA1SDQVrBwZV/wnyDAoiBv8v////DxEUCwgyEP8fDQeYCAklDA4REQ4TDAghBgljDxRBDhASCgcYCAklCxEh/////wX2BwopEBiFEv8fEAohDAsTDxFy////////GRM0EQlRF/8fDQSLCAoRDhIiCwkUD/9fExcVEg4iDhESExUhF/9PDRCyCQ80/xTxFRcVEhEhFxVREwsRD/8//xbxERMRFBYRGRcz/xLxD/8//xnz/xfzFRQR////GhgzDRJ0FRkxGv8f/w31EBVGF/8/////////GhdRFhQzGBcTGf9f/////w30uhjmeQEHQQZ9/aJhDFEPcV3aYQRDBINl/kEKWwqACQqiDkgIfmNSAgxVE33cbmIETAWC/3qiDC8ZflLG4gEhBIJyAUMPMSN4SiVDBz8IiSsqgxBFFXujNUMURgh6QVoDDUYSfjOF4w9ADIuxAkQQQRh4sgVkETdHcVwRpBM6FWlFOWQXIwpmJFokDToJfM1tRBMqO2cpikQLTAh987pEEzUYZacBRQ1EBnQgAf8D9gUCof////////8E8wMCIwD/T/////////8A8QEDNQoGowYCFQABYgQMFgUKNP8J+AUDIQH/P////wYCWQMBNQQMIwcKEQMHFwr/bwj/H/8C8wwJJBMKYgYFcQT/P/////8C8gYFFgr/fwoHZAT/jwwLMQ4NMf///wgGdgcJJg0Tdg4TJg0JIQT/jwwSNAT/X////xIRPw4LYxX/PwoHdQkLEg4PQg8VGA0HRwsMJv8Q8Q4MFxAUEhcThP8N8gv/LxEU8xYTRw8OERMQ/w4M//8S//8U/xYUExEM8v///////xf/PxUILQ0PFBAUU/8S8/8W8hcTcxARPxf/H/8I+w0TMhT/b/////8X9RMPExQSIRUUFxb/X////////9Ic6GlhB0YGfwGawQxRDnFd5iEERgSGYwbiCV4IhA0KAg9LCYFhWqILVxF/3mLCBFEEhQZyAg1FGIFVzsIBIAOEZ/nCDkcmd6EpAxRNCH1GKeMGQgiKLTbDEEwSez9m4wxKD4I6agMPNxaFNZFDED8IjLCqwxYwE3E/vkMXFBZztuLDETMSebby4w9BD4C18QMRKRx5cCWEEyUbak5RhBckC2cjamQNRQh+yGnEEyY2ZSuWZAtMCYDqusQTQxhmrfHEDEYGeFAB/wH0AwJh/////////wT0AwI0AP9P////////////AAMWBghDBgImAAFjBAclBQtECglYBwNCAf9P////BgJqAwFGBAcyCQtSAwUmCwhi////AgBECgkUCwY4BQEnBP9P/////wLzBgcpC/9/CwZbB/9P/wzxDg0yBP9f////EBIUDAky////CAZ2BQklDRd2Dw4jDQkxBP+fChA0Gf9PCwV3CQwjDhMzF/9fDQc4CQwzEA9xExkYDQ5BDAolEBJh/////xHxFhUfEgpRGBUvDxBh/////xbxDBAVERVf/xTxEw8xDxAYFBgSGxeF/w3zDxIRERVPGxeFEw4RFxL/ChH/Fv//GBn/GhgSFRHx/////////xvzGQg+DRMlGBoyERYi/xry/xfzFBUvG/8f/wj8DRdDGP9v////////GxdSGBYhGRgWGv9f/////wj7</t>
   </si>
   <si>
-    <t>9790</t>
-  </si>
-  <si>
     <t>Maryam</t>
   </si>
   <si>
@@ -220,18 +178,12 @@
     <t>TlQAEOgLAAAKAU5GVBDeCwAACgFORlIl1AsZAAFoAfwB/AEAAP+KAQEfAAAAB/8ZB5pxwBRJBnGXvcASUAdwkhGhDlcIcYkl4QZFCXGcbUEWOwZogMkBBU4JepfuIRJVCG2LieILVwmAdr2iBEkQe6LmghlEBmdy7SIGUxF8Gg3jDFoJgSQNQxdRBXSgLQMWUAV5eooDClEReZ2y4xBcBHujvaMVUwVxleqjDlcLdmxSBAw1H3hAaoQISSd3H20kCxtefRptRAstVH2fFoUVUAqCny1FGEcMeK82BQpLCYMGLAH///////8EBkgB/z////8A/z8EBiYC/0////8BBEIGBzoFA3P/////AvMGBxgF/18B/y////8JDEcGAkL///8DAlcHCkgI/38CATYE/08MCzkHA2EFAkoGCWUNCyT/CvT///8FBmkHCjL///8E/0//////EPYMBiH/CPIFB4QLDiQT/58PEhgOCkIHBkn/DfUXEIQNByQG/z8J/y8GBEgM/y8XEHMPC2X/CvQHC3QREhQT/08LBhoNEGMWGDsRDiIGDXP///8WGG4RD1MOCxQPECUWGBkS/z8TCBsOEUMQFoEYFVH/////CvkOEkEUGPH/GP//E/8OEf8SFf//GPX/FP8OC2oSFhIREBb/F/H///8YEnEQCVr/////////FvEUEfkW/3////////8BBCRxJAsABwAEAAD/G5lhIBRIB3WVrWASUgd1kQUhDlcIc4YZYQZBCHScXaEVNgdqfslhBEoIe5bigRFVB28JAYIEOAt4ioFiC1kIgXbBAgRFDn2h1gIZRQZqcfGCBVQRfhwVQw1cCYQkHaMXUQZznyGjFVAFenWKYwlPEnqcomMQXAV/o61DFVMEdZHaIw5WC3ldRmQLMjB3HXHECz4yfTp6RAhLIHsjfWQLI0N/LpoECzAlhaEKBRVSCYSgIcUXRwx6sSalCU4Kh0QB////////BAY4Af8v////AP8vBAYWAgM2////AQQxBgg5BQNi/////wLyBggXBf9PAf8f////Cg5HBgJB////AwJGCAc/Cf9vAgE2BP9PCgwZCANhCAn//////wX/Awb/BwL5BgplDgwTDwtz////BwjyDAsR////BP9P/////w3yDgYx/wnxBwjzDA8UFf+fEBMYDwtBCAY5Cg6EGRFzDggTBgoy////BgRHDf8fGRFiEAxk/wv0CAx0EhMVFf9fDAYbDhFjGBRGEg8zBg5y////GBptEhBTDwwUEBE1GP8vE/9PFf8fDxJUEBhiFBYf/xfyFhXzExIUERiC/////wv5DxNRFxox/xf/Ff//ExT/ERj/Gv8//xXzExZPGRhlEhEm/xnx////GhSCEQ1H/////////xjxFxI6GP+P/////////xaceSAVSgSMlsEAE1QHjZEV4Q5ZBpCKJQEHRwePmmkhFkIGf37J4QROCZWW9mESWQeHi4niC1QKonS9YgRMEZah6oIZRgKBcO0CBlQSmSUJAxdOA5EdESMNXAylny6jFkcElXOOwwlPF5ucugMRXgWdor2jFU8DkZHuww5VDZY5boQIRy+aoBplFVILobMqxQlMC6igLUUYSguZCAH///////8EBkgB/z////8A/z8EBiYCA0f///8BBEIGBzoFA3P/////AvMGBxgF/18BACT///8JC0cGAkL///8DAlcHCkgI/28CATYE/08LDDkHA2EFA0gGCWULDET/CvT///8FBmkHCjIS/78G/x//////EPYLByX/CPIFB4QMDiQS/58TDZEMB3QG/z8J/y8PEhgOCkIHBkkJDYUGCzEJ/z8VEHMPDGX/CvQHDHQPESES/08MBhoNEGMTFDsRDiIGDXP///8TFG4PDDIODBQPECUT/x8S/z//////CvkOEUMTFHEREBb/FfH///8UEncSERkT/3////////8QCVr/////////E/H/HJdtoBRGBY6WsYASUgeRkhGBDlkHkoYZYQZDCJKbXaEVPAaAeslBBEcIlZXq4RFVB4kJBYIEOQuRioFiC1UIo3PFwgNMEJeg1gIZRwKEcPliBVQTmiYVgxdTBI8fHYMNXAymnx4jFkkEl22KIwlDGZqbroMQXAafobFDFVADk4zeIw5VDphRSkQLHUeUOGpkChN3mB9x5As9L5g3gkQIQySfJoJECyZAmyqeBAszJp+hCgUVUQmjtx5lCUsMqqAd5RdLDJpQAf////////8E8wH/L////wD/LwQGFgL/P////wEEMQYIOQUDYv////8C8gYIFwX/TwEAE////woORwYCQf///wMCRgYHPwn/bwIBNgT/TwoNGQgHbwgJ//////8F/wMG/wcD9wYKZQ4NIwsJMv///wcG+QgLIRb/vwb/H/////8M8g4INf8J8QcI8w0PFBb/nxsRcw4IEwYKMv///xATGA8LQQgGOQoOhQYERwz/HxsRcxANdf8L9AgNdBASMRP/Xw0GGw4RcxkYSRIPMwYOc////xsZRhIQUw8NFBARNRn/LxP/TxT/HwsPlRL/TxUX8hoWIv8L+g8TYRUX8f8Y/xcU/xMS/xEZ/xr/H/8J+w8UUhf/P/8Y8RYUMRMSJhUZ9P8a8/8W8xcVH/8Z9RARRv8b8f///xoVjxgQPBn/j/////8J+xEKSv////////8Z8f8bnnXgFEAHXJa9ABNLB1yGCkEHOQhZkhXhDlEKWaGqIRcWA2KAyeEESglnmPZBEk0IWwQB4gMtB2WLiSIMVwlsdr2iBEgPax/aohsLBWtx6SIGUg9qpO6iGUAHXyQJIxdMB2IZDQMNVgdvojEDFkkHYn6KAwpADF+gssMQWQVlo8XDFU0FX5bqow5UC2F2VgQMJxtgPm5ECEkeXhhxZAs3V2YxkuQKMDdrnxqFFU0Ka50tRRhCDWCtMuUJTAluRAH///////8EAUMD/3////8A/z8EBiYDAkb/////A/IGCBgF/1////8B/08GCDoFAnIB/y////8MDzcGAzH///8CA1cIC0gH/y8DATYE/z8NDjkIBWMICSX///////8FAygHAyoGDGUPDiQQC3T///8HBlkICzL/////EvcMBhEE/z//////CfIHCGQOECQV/58E/z8K/x8ZEqYNBiEZD4IRCHQG/z8M/y8RFBgQC0IIBkkED8UGDUIM/z8YEpMRDmX/C/QOD0kTFBQV/08OBhoPEmMYFDUTECIPDTT///8YGm4TEVMQDhQREiUYGhkU/z8VEBQOE4MZGDEXFhH/////C/kQFEEXGiH/F/H/FfILELYUGBIa/y8VCS0QFmEY/z8TEhb/GfH///8aFHESDVj/////////GPEXEygY/3//////////G5tpgBRGB1+VsYASTgZgkglBDlIJXYoOwQY4CVyfmsEWIwVifclhBEgIapjqwRFQCFwGAWIENAlnioWiC1gJbXK9IgRJDGyi3kIZQwlgc/GiBVMPbCUVgxdOCGIbGWMNWQdxoB2jFU4HZHuKgwlODWCfpmMQWwVpo7WDFU4EYpPaQw5WDGRoSoQLMyRgHXXECzo0Zzt+RAhMGWMnikQLJkVqL54kCzMlbaAOJRVQCW2xIoUJTglzoCXFF0UMYkQB////////BAZIAf8v////AP8vBAYmAgM2////Af8/Bgg5BQNi/////wLyBggoBf9fAf8v////Cg5HBgJB////AwJWCAs3B/8fAgE2BP9PDg1JCANiCAkU/////wXxAwZ0BwIZBgplDg0TDwtz////BwZJCAshFf+/BP9P/////wzyDgZB/wnxBwhTDQ8UFf+fGhFzDggTBgoy////EBIUDwtBCAY5Cg6EBgRHDP8fGhFiEA1k/wv0CA10EhMVFf9fDQYbDhFjGBRGEg8zDgwj////GBluEhBTDw0UEBE1GBkqE/9PFf8fDxJUERiCFBkS/xbx/xXyExIUERiC/////wv5DxNRFhkx/xfxFf8/ExQhERik/xnzFQk9FhQSGP9fEhEm/xrx////GRSCFxI6GP+P////////EQpK/////////xjx</t>
   </si>
   <si>
-    <t>1234567</t>
-  </si>
-  <si>
     <t>BSN1234567</t>
   </si>
   <si>
     <t>TlQAEI8MAAAKAU5GVBCFDAAACgFORlIlewwZAAFoAfwB/AEAAP+ZAQEfAAAAB/8fBwoK4AklBowFKgAFNgN6hk3gCVEJiYiZYA1UCYp94cAFUQh8kupgFkoDewbyoApZBYONBQETUwSHcRahARMLfIEZQQtWBYUEWmEIOQaGf4VhCkIGhY69ARRQA4VwzSEFRweKEukhFE0Eio1VAhNbBpOTWgIYUwSEGd4iGE0FgYLhAg9PCpcGBaMMUgeWhiaDEFkJj2Q1wwEiCI6XTUMXUwSD5J6DAkcIj2/Z4wtUEojuOmQIVQyImILEFUwFhg2OBA1DF3prkqQLQxN968JkB0MLg/fhZAkyDoMGdAEDAjIEAXH///////8CBBUI/2//////APEBABL///8DBiUECFYC/y////8HDikGBDP/AfUAAnUGChQNCHEA/x//////DPYLB3IMCTEKBDEBAlUDBzED/y//BfL/DPUTCeP/////AfYEDRYV/+8EBiEDB1MMDzgLCkILEhwN/z8IBDQGCTIKBBYJB0YMEhsVDaIJBzUF/28QDjISC7H/CPYECnMLEywV/58QDxQSC6IJDFL///8LDFUOEEIRGi0SDWQOBRj/////EfMUD4L/FvMUElQPECP///8NC6sPEWQWFBIYE5IUGBcZFYQNC80PEoITEhIPEXUWGiYYF2L///8IDekTGFoX/z8PEVP/////GvgYFIITGScd/5////8VDTsXFWoTFHYWGoEbGVEaHCMd/y//F/cNGOEUFmj///////8eG1P///8eHBEZGDUWGsMdGRMYFFob/x//HvEcHhL///////8ZGCT///////8dFywZHFEABAAHAAQAAP8eCg5ACiUFjQYqgAU4An6GSWAJUQeJhZHgDFQLinvdQAVRCH2R3uAVSwV/BvYgC1kFhY0BgRJTBIp/FcEKWAWFBVoBCToGiHyB4QlBB4aMsaETUAOFbsnBBEcHixPxgRRQBYuKTaISWQeVk1KiF1MEh4DZgg5PCZgZ6qIYTASDCgkDDVgHl4oiAxBSCZFbPWMBIQmOlkHDFlQFheaS4wJGCZBr2WMLVxGL8S7ECFYMiph2ZBVMBYgQkqQNRBV7apYkC0MRfu265AdECoP63eQJPRGDaAEDBjcCASL///////8CBBUU/+//////APIB/x8A/y8DBhUE/08CABP///8HCxYGBDL///8BAlQICRQM/28A/y//////C/YKB5ILDjgIBBEBAmUDBzED/x//BfL/C/QSBuEEAhYGBxILDicJDCULChEM/z8EAkgIByT/CfEIBzULEBoUDJEIByQF/28PDTEQCqH///8ECWMKEBkU/48PExsOCjELBxf///8KC0QNDzIRFSQQFFUNBRn/////EfQTDpIMCpoOD1cVExIXEoH/FfMTEGQPBUz///8TGhsXFmIMCrwQFREQCi0OFXL/GvsXFmP/////DPgSFzkW/z8OD0YR/z//GfgXE3ISGCgc/6////8UCjz/FvYSE2YVGXEbGFEZGzQc/z//FvgMF+ETFXj///////8dGlT///8dGxEYF0UVGcQcGBQXE1sa/x//HfEbHRL/////FvoYFzT///////8cGCUbGhH/GAcmAAU3BZmGScAJUgishZHgDFULsXzh4AVQB6CR5mAWSgOdB/bAClkGqY0FoRJUA61/GUELWQeqjaoBFEcDqG3CgQQ+B7AU7YEUUASvilGCElYHupVe4hdVA6h9zkIOQAu/GeJiGE4FpAsJAw1TCb2EHmMPWQu4lkkDF1QFp+eawwJECLFq3YMLVhSx8zakCFMOrJd+ZBVNBanuxSQIOg6i/OWkCTwWoSABAQMV////////////AP8f////AgUlA/9fAf8v////BgopBQMz/wD1/wH1BQsaCf9v/////////wj1DQbiCAchCQNRAAFVAgYxAv8v/wTy/wj0DwfjAwUhAgZjCAsoEgnkBwYkBP9fDAoyDQmi////AwdlBg2JEv+/DBEYCwlDBwhS////BwaKCgxCDhElDf9fCgQY/////w7zDQti/wn5CAulERASDxIh/xHzEA1TCwwj////EBMXFBKCCQfODREjDw0SCw51ERUmExJiCw5T/////xX4ExCCDxQnFv+v////CQe+/xL2DxB2ERWBFxRxFf8vFv8//xL3DxOBEBFo////////FxNRFRdi/////xL6FBM1////////FhQlExV1/xoJKoAFOAOci0kgCVIGq4SNIAxVC7CR3uAVSgOgfOFABVAIoAn2QAtaB6qL+QASUgOxfRmBClgHqIuigRNCBKlvygEEPgayFPkBFU8Er4hFAhJWCLuTTkIXVQOrfM7CDUAKwBnuohhKBKQKDYMNVgq9jh7DDlgLuZRBwxZWBajpikMDRgiyZ+HjClMTs/cqJAlVDq6VbgQVTgWrEZKEDUUYnnCi5ApCF6HyvYQIOg+iA9lECjYYoTgBAQQV////////////AP8f////AgUVBP9PAf8f////BgoYBQQy/////////wj2DQbi////AAFUBwsZCf9vCAs4BwQRAAFlAgYxAv8f/wPy/wj0DQXhBAEWBQYSCAsnEgnkBQY0A/9vDApCCwlT////BAdkCw1KEv/PDBEXCwkyCAMn////BwZ5CgwyDhEkDRJXCgMZ/////w70DQty/wn6CAu1ERATDxIi/xX7ERA2DANM////EBYbExJiCQ3CCxFhDw0TCxFyFRZ7ExJiCwxGDv8//xX4ExByDxQoGP+v////CQvH/xL2CQ/mERVxFxRRFRckGP8//xL4DxOBEBF4////////GRZU////GRcRFBBLERXEGBQUExFcFv8fGf8fFxkR/////xL6FBA7////////GBQVFxYR/xuFScAJTQlthpEADVIKcXzdwAVOCWSS6mAWRgZlBfagClMGbY0BoRJRBXCCGSELVAdvBVqhCDcIcYCFQQpACG2QveETTARrb83BBEYHcRLtYRRPB3CNVeISWgd5k1oCGFEFbYXhIg9OCX0Z4kIYSgVqBAmjDFMGeYYmYxBWCXaWSUMXUAVr5I1DAj0Jd2/ZowtTD3HtNqQIUgtumYLEFUkFbwuOBA09FWtrksQLPw9r58ZkBz8LavT2xAkrEG1EAf///////wEEJQL/XwD/L////wUJJwQCM/////8A9QQHFAr/f/////////8J9ggFcgkGMQf/PwIAFQEFMQH/L/8D8v8J9RAG4wIEIQEFUwkMOAgHQggOHAr/P/8C9AQGMgcCFgYFRgkOGxMKwgYFNf///w0LMg4Isf///wIHcwgQLBP/vw0RGgwIQgYJUv///wgJVQsNQg8WLQ4KZAsDGP////8P8w4McgoIqwwPZBIREhQQkv8S8xEOVAwNI////xEXGxQTcv8I/QwOghAOEgwPdRIWJhQTYgwPU/////8W+BQRghAVKBn/r/////8K+xP/fxARdhIWgRgVURYYIxn/L/8T+AoU4RESaP///////xoXU////xoYERUUNREWoxkVExQRWhf/H/8a8RgaEv///////xMVohb/X/////8Z8hUYUf8bhUlACU0HbYWNgAxSC3GR2sAVSAZqfN1ABU4JZgnuAAtVCG6O/SASUAVzgBWBClUHbwVaAQk2B3J/gcEJPwhvjK1hE0oFbW/VQQRGB3QS+cEUTwdxjU1iEloHfJRSghdSBHGB2cIOTgh+GerCGEYEbAgJAw1XBnyJHsMPVgh6lkHDFlIGbuOJwwI+CXhs2SMLVQ127yoECVMLcZh6ZBVJBnEMkoQNQBRsa5pECz8Obeq65Ac/CWz86gQKMRFvRAH///////8BBBUD/08A/x////8FCRYEAzL/////////CfYIBYL/////APQGBxQK/28JDj4GAxH/APUBBTEB/x//AvINCXQIBFEDABYEBRIJDCcHCiQJCBETCtMDAEgGBST/B/EGBTUJDhoTCrEGBSQC/28LDBQOCKH///8DB2MMEDsT/68NEhcMCDEJBRb///8ICUQLDTIPFi0OClMLAhn/////D/QODHIKCJoMDVcSERIUEIH/FvsSETYNAkz///8RFxsUE2IKCLwOEhEQDhIMEnL/F/sUE2IMDUYP/z//FvgUEXIQFSgZ/6//////Cvr/E/YQEWYSFnEYFVEWGDQZ/z//E/gKFOEREnj///////8aF2T///8aGCEVFEUSFsQZFRQUEVsX/x//GvIYGhP///////8TFaP///////8ZFTYYFyI=</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>anna</t>
   </si>
   <si>
@@ -244,9 +196,6 @@
     <t>TlQAEF8LAAAKAU5GVBBVCwAACgFORlIlSwsZAAFoAfwB/AEAAP+ZAQEfAAAAB/8ZB6ueIAlICH8o7WAMTQSDqR4BD0wEeaXaQQtOBZoj/aEITQSfov0hEEcIdZ5xwg4YCHijdoILUAaFl4WiEB0HcRGlAhMRBm+lrQIJTQWHkdqCFREKch3lwghLB4ibWQMNTQmDo2ZDCE8KkJKtwwxYCoiIwkMQSAl7ms5jB0MKjwoBZAZDCIuLDeQJVgiNfRIkEUcJgmUVJBQhInuIToQKUQqCc1kEEyglhIl+5AdHCYMGLAH/////AfID/z////8DBFn/APL/////AvH///////8FAzb/AfEAAjb/BfMHCjcE/z8HERz///8AAXkDBjIC/z////8IBjQHA2MDBRT/CPEQDXYKB1IEAhkGCCINDEQK/z8DBRP/CfEVDfYMBmELEBcNCGEFAjX///8EA0cHEDMNDCL///8J/x//////Ff8QB2ENDhP/////CvIGC2UMBhYJ/28QDyMRDmMEDIMNDzETEUP///8ODRMJEIEUFjUTEUMNCCcL/28VFPIWD0H/DvMPEDITEhL///8WGBP/////BP4REyERDhQPEEP/FvIYEkEPEDIL/48VF/P/FvEUEP8JC///////F/8SExIPFFH/////GPEWFCMLFa//////////EvMTFkH///////8ABAAHAAQAAPYdqY7ACEUIgyf9wAxPBISpCqEOTAN9msqhFRcMa6fS4QpRBZuk7aEPSQZ5JgkCCVAEoJ5hYg4lCH2maiILUQaMn3UiEB4HdKahoghRA4wYsaITEgVwmM7iFBIHcx3xIglNCIeESUMUGQ53nU2DDE0JhaRaAwhRCpGTpUMMVwqKicKjD0wKfZnG4wZBCo8JCeQGSQiOjQlkCVUHj4AahBBKB4Z2OqQSIB+Di04EClIKhHVlhBIlI4eAekQHRQqHcIrkEgwhh26uRBIXHIZcAf////8B8gT/T////wUEFf8A8v////8C8f////8D8QUENwEAEwL/H/////8L9QUENwABRQMFcwgGQ////wL/PwP/PwkHIwYEUwgTHP///wAEcwUHUQQFEwMJYQ4P9QgGIQYFFgcLIg8NRAr/PwX/LwMLUQ4P9QoHQQYENwgSNA0TGf///wwOHw8JUQUDJf///wsDFv////8O/w8JUQ8QE////woIFAcOXwgL/wz//////xYS/w0HFQsOXxIRIhMQYwAN4w8RMRUTRP///xAPEg4S8RYYNRUTMxEJFw7//xcWQxgVU/8Q9A8RYxUUEv///xgaE/////8T8g8VcRMQFBESMxsYUhoUQRESMw7//xcZI/8Y8hYSJA7//////xn/HxQVEhEWUhz/X/8a8hgWIxf/H/8b8Rz/L/8U8xUYQhz/T////xgWRRn/H/////8c8RoYRRkbIf////////8ZrJogCUcHoSfxgAxRAqWqGuEOTgWbp8bBClAFuqT9QRBLCo4kBeIITwK7oj0iDi0Jl6VmAgtRB6ecboIQJAiBpaGiCFIFrRvpwghLB6ukVsMHUQuznFkjDU0Lo5atgwxYDK6LwiMQSwugncrjBkQKrwgFBAdKCauLCWQJVguugBbkEEgKoopOhApUC6VyaiQTKySRiX7EB0cMoWWaBBQSGIpyyeQRGxmLcQbFEQcWiiwB/////wHyA/8/////BAMl/wDy/////wLx////////BAM2/wHxAAE1/wbxBwUz////Av8/////CAYjBwNjBwsX////AANzBAZjAwIWBAgxDgqHBwUzBQIZBv8/DApECf8/AwQS////FAzGCQZRBQNHBw4zCgsk////DAsT/////wnyBv9/AArjDA0xEQ9D////CggW////Dg0jDwtjCwwT/w7xEhM1EQ9DDAgn////FBJSEw1B/wvzDRExExAy////ExUT/////w/yDBGBDwsUDQ5DFBNCFRBBDQ4y/////xTz/xPxEBESDRJRF/9f/xXxExIjCP/P/xbxF/8v/xDzERNBF/9P////FxMUFP8f/////xjxFRNFFBYh////GP8fFRNWFxYR////////7husgqAIQwejJwHhDFECpaoKwQ5OBZynwmEKUAW7nMqhFRsLgqbtwQ9NCJMnEUIJTgO6oi2iDSQInqlWggpKBq2XYuIPJQmGppVCCEgDrx3tIglLCKqkSoMHUQuznVGjDE0LpJWhAwxXDLCWvoMGQQqvicJjD04LopEFxAhTCq8GEYQHSwmsgRpEEEwJpnYhpBMPJJJ0OWQTIyWTjU7kCVALpnVy5BIkI5J+fiQHPw2hYqJkExMei3TVhBEbFoxEAf////8B8gP/T////wUDFf8A8v////8C8f////8E8QUDNwEAEwABRQQHcQgGQ////wL/H/////8N+gUBMQL/PwT/PwkHIggDYwgKE////wADcwUHUgECRgUJIRALhggGMgYBGAf/Pw0KQ////wcFEgT/XxQN9gsIYwAIowcUXwsMFP///w0ME////woIFAn/bwAL4w0OMREPRP///wsJFv///xAOIg8MYwwNEgQQwRMWNREPM/8M9A0OYxIYJf///w4JGAT/zxQT8xYRUw8MFA4QMxb/LxgSQRYYE/////8P8g0RcQ4QMwT/7xUX9P8W8hMQ/wX//////xX//xMQ/xT//////xf//xIREg4TUhr/Xxj/LxYTNBX///8Z8hr/L/8P9hIWMhr/T////xoWFRcUL////////xgWRRcZIf////////8VrqIgCUYJaSnxgAxJB2upGuEOSQVmpNpBC0wGfiP9oQhKBoOiAUIQQQdponaCC0wFcqapwghMA3Ef5cIIRAhtmVkjDUoJbqJmQwhNCXeSrYMMVApviMZDEEQJZ5vOIwc/C3YLBcQGQwlyjBHkCVIGdX0WJBFDB3VlFUQUKyBwhU7ECkwJaYh+5AdFCXDyIiUODQN//AD/////AfID/z////8DBFn/APL/////AvH///////8FAzb/AfEAAjb/BfMGBzcE/z8GDRz///8AAXkD/z8C/z////8MCMoGA2MEAhkF/28JCEQH/z8EA0cGCTIIDSj///8LCjP/////B/IFCaEIBRr///8MCyMNCmMECIMJCzEPDUP///8KCRP/DPEQEjUPDUMLBhX///8REPISD0P/CvMLDzESDjL///8SExP/////DfIKD1ENChQLDEP/EvITDkELDDIF/+8R//8UEnEQDP8G////////FP8ODxILEFH/FPb/E/H/DvMPEkEU/1//////////////EvYQEX//Fq6SwAhECGwp/cAMTAZtqQqhDkoEaafOwQpPBoCk8cEPRAZrJQkCCU0FhKZqIgtNBXennYIITwN0HvEiCUkJboBJgxQWDmucVaMMSglxpFrDB1AIeZKlIwxTCXGHvqMPRwtomsbDBj4MdnX1gxQgHnCKCYQJUQZ4CQ1EB0QHdX8apBBEB3R2PsQSLB92iVJECkwJbIR6RAdDCXQIAf////8B8gP/T////wQDFf8A8v////8C8f///////wQDN/8B8QABRf8E8wYFQ////wL/P////wkI+QYDYwYLGP///wADcwQJXwUEFv8J/woIRAf/PwUDNwYNNAgOGP///woLE////wcGFP8J/wYE/////////w8N/wgEGf8J/w0MIg4LYwAI4woMMRAORP///wsKEv8N8RIUNRAOMwwGFgn//xMSQxQQU/8L9AwNMxEVJv///xIK/wn///////8T/w4LFAwNM/8U8hURQRQVE/////8O8gwQQQwNMwkP/xP/L/8U8hINJAkP/////////xEQEgwSUv////8V8v8R8xAUQv///////w==</t>
   </si>
   <si>
-    <t>40</t>
-  </si>
-  <si>
     <t>Kirana</t>
   </si>
   <si>
@@ -259,9 +208,6 @@
     <t>TlQAEM8HAAAKAU5GVBDFBwAACgFORlIluwcZAAFoAfwB/AEAAP+jAQEfAAAAB/8SB5/GoBIpAoSX8WALSwh1lGFBBDoHdphhoRFJCIYWisENTwOCktnhClIHepllghVEBIoTdiIMUQOLHnXiE0YEi5OqIhFHB5AR/iIIUQSVoP6iF0EGgpopwxQqBYWbPoMUKwWEJ8WjFE4GjSX6AxBTBoiZEcQKSAeAo1HEE0sGkAbYAP///////wYDhAH/X/////8D8QQFNgL/b////wEEYwUKGv////8A9P///wgHegQBMQgHNgUCMwH/PwP/PwIBFgQGMgkHNP///wP/X////wsMLwgHJQwP+Ar/XwIFVAMJoQsPHAkHNAP/fwb/LwUDOQgLMgwP+RAH0Q8QJv////8F+QcJVgb/L/////8O9gwJ8gkI/wv///8N/w8H/wkMHwv/P/8O8w8Hcf8R9A8HVA0LNv///////xAKQgkNlw4RUQoJbQ4PlP///////wkOhP////////8P8QAEAAcABAAA/xEcpcASCAOKobpAEioChJjlwApMB3eZUeEDNQV4mFEhEUsJhheSIQ5RA4SRzWEKUgd8mFkiFUgEixJ+ggxQBI4kgWIUQwSMkqKiEEYHkqLuQhdDBYUSBqMITwWXKdEDFU0GkJgBRApFBoUmBmQQUQWKoUFkE0sGkswABwH/Av///////////wD/////BwSEAv9f////AATxBQY1A/9f////AgZRCP9f/////wH0////BwhKBQIxCghnBgMzAgE4BP8/AwIVBQcxCgg0////BABP////CwkhCghVDQ5MDP9vBgVHBAqhDQ98CgYxBQcx/wvxBgU2BwlTDQ9aDAhxCf8f/////w32DAqTDw42/////wb5CAlq/xDzDwhUCQt2////AwzmCw/k////////////DgxDCgurDRBRCg2D/////////w/x/xGftiASKwSemPnAC1AIl5RdQQQ7BZaYXYERTQeoF44BDlMCo5LdAQtVB5+XVQIVSAStEoKiDFMEtiGBQhRGBKyStYIQQge5oPqCF0QEoxMKwwhSBMCZJYMUOgapKtUjFU4GsScKZBBTBqqYEYQKSgeioEWEE0oGscwA////////BgOEAf9f////AANRBAU2Av9v////AQRjBQ8e/////wD0////BgdaBAExBgcWBQIzAf8/A/8/AgEWBAYyCQdE////AwBY////CggiCQdVDA8cC/9fAgVUAwmhCg4cCQVCAwZy////BQRGCApDDA4ZDwfRCP8f/////w32DAkzDg8m/////wX5BwlWCQgUCv8//w30DwfB/xD0DgdUDApG////////DwtCCQyYDRBRCwltDA7E////////CQ2E/////////w7x/xGkruARKwSfl+lAC1AHmJBNwQM1BZiaTeEQTQimF5JBDlQCpZLVgQpSBp+XTaIURwSvEIYCDVIEuCOJohRDBayPqSIQQga6pO4CF0UEpBMOIwlQBMGXFQMUOQasLOVjFUsGs5YBRApIBqUoEsQQUwaroDkkE0oGscwA////////BgOEAf9f////AANRBAU1Av9f/////wH1BQsa/////wD0////BgdKBAExBgcXBQIzAQA4A/8/AgEVBAYxBwtJ////BAAY////CgghCQdFDA4cC/9vBQRHAwmhCgwTCQUxBv8f////BQQ2BghDDA8ZDgfBCP8f/////w32DAkzDw42////AgWpBwxlCQgTCv8//w3zDgu1/xDzDwdUDP8/////AgvmDA+0////////////DgtDCQyYDRBRCQ1z/////////w/x/xCY9YALRglflVLBBDIGYJddgRFGCWwWjuENTQRvktnhCk4IYphdQhVDBnISemIMTwVzHX0iFEUFcpWqIhFGCHOf+qIXRAdrEf4iCE8Fepw+oxQ5Bm4oycMUTQZzJAJEEFIHcpkRxApFB2ijTcQTSQZ0wAD/////AvEDBDYB/1////8AA1IEChr///////////8FBloDADEIBlYEATIA/z8C/z8BABYDBTIIBjT///8C/1////8JCyYHBiULDRgK/18BBFQCCKEJCxQIBjQC/38F/y8EAjkHCTILDRkOBtEH/x//////DPYLCDINDib/////BPkGCFYIBxQJ/z//DPMOBrH/D/QNBlQLCTb///////8OCkIIC5cMD1EKBmwMDZT///////8IDIT/////////DfH/EJfpAAtHCGGZSkEELQZjlk0BEUYJbRiSQQ5OBHGRzYEKSwhkl1HiFEUGcxOCwgxOBXYgiYIURAVzlKaiEEcIdqHuQhdFBm4SAmMITgV8mjJDFDgGcSrZIxVOBnaZBWQKRQdtJQqEEFIFdKI9ZBNJBXjAAP////8C8QMENQH/X////wAEUQb/b////////////wUGSgMAMQUGFwQBMwD/PwL/PwEAFQMFMQYKSf///wP/H////wkHIQgGRQsNHAr/bwQDR/8I8QkLFAgGNAMFMf///wQDNgUHQwsOKgoGcQf/H/////8M9gsIQw4NNv////8E+QYIZwgHJAn/T/8M8w0Ktf8P8w4GVAsJNv///woGbAsOtP///////////w0KQwgLqAwPUQgMg/////////8O8Q==</t>
   </si>
   <si>
-    <t>41</t>
-  </si>
-  <si>
     <t>Rara</t>
   </si>
   <si>
@@ -269,16 +215,76 @@
   </si>
   <si>
     <t>TlQAEAkKAAAKAU5GVBD/CQAACgFORlIl9QkZAAFoAfwB/AEAAP+pAQEfAAAAB6gdB7E6QAsdBZuwdeAFHBB+vJUADjQIo0Py4AQsCnTGBqEQKwO8yDHhBCAQfcdJQQxJDZDFUaEOHgao1HaBAxQLddSFgQY9CnTJjkETNQKtWrlhCjYGhFbxgQ4cCZ3W+aEJNQaBzxLCDi8KnOEaQgU8DHLKLeIVMgK0XDXiDSwUltBVIhAlCp9baeIOHxWZz6YiDxcLl3CyAgcoCIRQssIXIASr5x6DBiILidAlYxYWB6BZLqMVHgie5U0DDDYFiPn6wwUQBYPrHuQMJwyCBlwB/////wLzBgMWAf9v////AAZnA/8f/////////wT0BgMpAQCTCP8f////AQIZBgVx/////wr0BwYlAAJkAAZnCwlzCP8f/wPxAgcjCgyFCwkUAwBxBP8vCgxjDQYjAwKiBQkSDxc6/////wPxBgtEDQ9S/wjyBQEz/////xD1DAtZBwRkDwkUBQZxBww1EQ1hFQsVBgdTChBaEg5BBxElExVz/w/yCQtRChA4EhMhEQ0VCwxhDREmFf9P////CAky/////xb0GhI2DAqlFQ0lCw5hChJTExolChAWGRyZExUlDgcmFQ1HEQ4hEhYqGRShEhYYGRyIGhUlDROB////Dw1DFBpXF/8vGRIZEP9P/////xjxFBokG/9v////FQ0l////////HBkhFBaRHBQYEhaRGP8f////Gf9vHBtj/xf0DRSiHP8v////////Fxpj////////GxcpGhlhAAQABwAEAACaITcmQA0SBZ2xZaAFGBGBtIUgDjMIpcT24BAqA75EBgEFLQt6uR0hBSAOfcQ5gQxHCpTFQcEOHwSr1mbhAxYOedF1AQc9DnnJfmETOQKuU4FhDxIHqVWKwQ4kCqRhxQEKNQaD2O0BCjUHhF39QQ4nC5vMBiIPMQee4gqiBT4LcssdAhYxArdfPcINLBSW0EViECYIoF51wg4YE5jMloIPGA2ac7qCBicJh026ghchA6zoEuMGJAmIzBnDFhYFpFs6YxUeCJvjRYMMOASK05njExQGhWWlQxMcCIT2+kMGEAeG6RpkDSkJgowBBgEY/////////wLx////AAaGBP8f////AP8f/wP0BgQZAf+P/////wr1BwYlAQLECP8f////AQIZBgVxBAIYBgliCP8f////AgMVBw8kDQkTBf9vA/8vCgtvDQklBgIhAgmCERdI/////wXxAgZTDREy/wjyBQEi/////xL1EAtPBwNlDAn/Bgf//wr/Eg//DQk2BgcxCwr2Eg+hEQkTBQZhDA80DhcUDA8jExdD/xHyCQ1BFw4TBgxBChBRFBMhChJIFBUhEw8RDQxiDhMmF/9f////CAlC/////xj0HBQlCwr1Fw4kDQ9RChRSFRwUChIVGBaRFRMSEAwkFxFIExARFBgaFhwSFBgZGx2fHBcmFRAS////EQ5TFRxHGf8/GxYZFBKU/////xrxFRwUH/9/////FxMx////////GxwWFhiRIBwmFhiRGv8f/x3/Gx5vIB9j/xn0DhaSG///////Hhz/FhT/IBz/Fhv/Hf//////IP8/////////GRxzHv//////Hxk6HBthpw5F+uAQEwm9wz1hDEIOscxZIRMiA8FYjuEOIwu8056hBjIIj8z6IQ8tCbJfEQIOJA+p4h7iBDYIil9SAg4hD6rQUqIPIAmz5wGjBiUJpOJBoww0BaVnqWMTGwqW6hoEDScKnqgAAwEU/////////wLz/wD1AwU1BwQT/////////wz6BQM1AP8/BwQ1AQAxAv9fDAXhAQM1Bgdx////////Av8//wnxBgcVBANxCgQXAQNRBf8fCQghBghWCv9v/////wTxCgQYAQZR/wnxDAu0Av8f/wvzCgghBgUhCQslDf+v////Bwhh/wz3Df9v/wr1Bwi0DQsXCf+v////////DP8f/////wr6CwJqhxPBAYEOEAe8SAoBERQJwcUpgQxCDbPFSYETGQXA0FnhAg8UetCGIQcyDJNMhgEVCQO8WZahDiMMucvqYQ8uCLbhDmIFOQmLYSGCDSwQp88+4g8iBbZhYqINGg2o5QEDByUJpeExAw00BaZVRaMVFQmu1Y1DFBMKmmixAxMbCpfpEqQNKgid5AD///8BB/8KAv////8HAC////////8DCzL/AP8DB3MJBRP/////////BvIIBzUB/z//Bf8KCf////////8CBzYKDXgJBC////8IB1cD/y//////D/8JBVYCAD8DBlcICiEDBjX/C/IKCRYFB4IHClUN/2////8EBfL/BfgCB0EICxIMDhUG/z8PEP8MCiIFCMINCRcKCBELDy8QDvQMDhQS/6////8JCmH/EfYS/2//DfQJDLQQDv8LBv////////8P//////8RDv8LBv8SDhYMEL////////8R/x//////DfoOD2+wErdJwAoeBIOsiqAGHA94u5kgDjQHjE3qYAUuB3jFFQERLQOdxlFBDEcLfNeJYQY3CWLGnkETMgWPWb1BCjUHcdb9oQk0B2vjCcIELA5nzTnCFTIDlVKlghcjA5BwsgIHKAlwcFaDChYIeuRaYwwoB3bxbQMIFAZ7aImDDRYHcdgA/////wL/BQH/////////AAX2BgMh/////////wT1BQMpAQCP////////AQIZBQZz/////wf0CQVWAAL1AgQmBw6aCAYUAwB/BQhECQpS/////wPz/////wv1DwhLBQSUCgYkAwVxBAdrEQnhBwuuEQ3T/wrzBghRCQs+Df9f/////wby////DP9PDwk+BQflEQleC/9P////////////CglTCw7GEP9vEA0WCQuUDxET////DP9fEf8vEA4hCQujDv8f////////DQxoEA9CCQzW////////1RK4iSAOMwiMSvpABSwFe8UJIREsA5/IOeEEHhB7xUGBDEcIf9J94QY4DWPIjkETNwWQYMnhCTYHcNnx4Qk0CG/hDSIFLg5nzCniFTQCmVKxYhcjBJRyusIGKApz5/1CByQIcuZOwwwrBnh3XkMKFgd782ljCBUGfG2ZQw0WB3DYAP////8C9AQBGf////////////8A+QQDf/////8G9AcEVf8A9P8E/wUJ//////8B/wACFQYOmwcFEwH/fwAEUwcJMf///wP///////8K9Q4HWwQClAkFEwEEcQIKXg4IsQYKrQ4Mown/LwUHQQgKLgz/X////wMF8f////8L8w4ILQQG1Q4IXgYKk////////////wkIUwoPxw3//woP/xD//////wwI/wv/XxH/Lw8NLwgKohANHwgLlw7/L////w//H////////w0L9xAPMw4LI////////w==</t>
+  </si>
+  <si>
+    <t>CECEP4224</t>
+  </si>
+  <si>
+    <t>MULYANI4504</t>
+  </si>
+  <si>
+    <t>RUSTY3694</t>
+  </si>
+  <si>
+    <t>NURLELA4298</t>
+  </si>
+  <si>
+    <t>LIDIA20153</t>
+  </si>
+  <si>
+    <t>ANNISA6735</t>
+  </si>
+  <si>
+    <t>ANNASTASYA20703</t>
+  </si>
+  <si>
+    <t>Maryam9790</t>
+  </si>
+  <si>
+    <t>anna30</t>
+  </si>
+  <si>
+    <t>Kirana40</t>
+  </si>
+  <si>
+    <t>TIURLAN3947</t>
+  </si>
+  <si>
+    <t>EKO4670</t>
+  </si>
+  <si>
+    <t>ANGGIA13424</t>
+  </si>
+  <si>
+    <t>SRI4014</t>
+  </si>
+  <si>
+    <t>Frisilia4015</t>
+  </si>
+  <si>
+    <t>MUHAMMAD16027</t>
+  </si>
+  <si>
+    <t>RARA41</t>
+  </si>
+  <si>
+    <t>UserLDAP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -620,13 +626,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -640,316 +655,374 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>4224</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>4504</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3694</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4670</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3947</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4298</v>
+      </c>
+      <c r="B7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>13424</v>
+      </c>
+      <c r="B8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="C8" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>4014</v>
+      </c>
+      <c r="B9" t="s">
         <v>29</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C9" t="s">
         <v>30</v>
       </c>
-      <c r="E7" t="s">
+      <c r="D9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="E9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" t="s">
         <v>32</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>4015</v>
+      </c>
+      <c r="B10" t="s">
         <v>33</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C10" t="s">
         <v>34</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>20153</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>6735</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>16027</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>20703</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>9790</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1234567</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>30</v>
       </c>
-      <c r="E8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B17" t="s">
         <v>54</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C17" t="s">
         <v>55</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D17" t="s">
         <v>56</v>
-      </c>
-      <c r="D13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>66</v>
-      </c>
-      <c r="B16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" t="s">
-        <v>72</v>
       </c>
       <c r="E17" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="F17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" t="s">
         <v>74</v>
       </c>
-      <c r="B18" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>79</v>
+      <c r="F18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" t="s">
         <v>81</v>
       </c>
-      <c r="D19" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" t="s">
-        <v>82</v>
+      <c r="F19" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>